<commit_message>
added functionality for viewing Pega System Scan Result zip file
</commit_message>
<xml_diff>
--- a/src/main/resources/AlertMessageList.xlsx
+++ b/src/main/resources/AlertMessageList.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_PRIVATE\_WORKSPACE\MeshGit-LogViewer\pega-logviewer\logviewer\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_PRIVATE\Github\pega-logviewer\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1285" uniqueCount="589">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1360" uniqueCount="619">
   <si>
     <t>Id</t>
   </si>
@@ -1757,18 +1757,9 @@
     <t>PEGA0091</t>
   </si>
   <si>
-    <t>member unexpectably disconnected from the cluster</t>
-  </si>
-  <si>
     <t>member has disconnected from the cluster</t>
   </si>
   <si>
-    <t>Segmentation detected</t>
-  </si>
-  <si>
-    <t>Data lost detected for cache</t>
-  </si>
-  <si>
     <t>This alert is generated when the packaging time for a single database query exceeds the threshold setting. Packaging time is defined as the time elapsed from the execution of a query until the last row of the result is returned to the PRPC engine.</t>
   </si>
   <si>
@@ -1794,6 +1785,105 @@
   </si>
   <si>
     <t>https://pdn.pega.com/node/1318426</t>
+  </si>
+  <si>
+    <t>PEGA0092</t>
+  </si>
+  <si>
+    <t>PEGA0093</t>
+  </si>
+  <si>
+    <t>Distinct Values query time above threshold</t>
+  </si>
+  <si>
+    <t>com.pega.pegarules.data.internal.rd.SqlReportExecutor\ncom.pega.pegarules.data.internal.rd.SQLExecutorResultsCP</t>
+  </si>
+  <si>
+    <t>com.pega.platform.cluster.internal.util.ClusterMembershipManager</t>
+  </si>
+  <si>
+    <t>2 (DSS - cluster/data/backup)</t>
+  </si>
+  <si>
+    <t>PEGA0095</t>
+  </si>
+  <si>
+    <t>Raise an alert when the IH aggregated data is not up to date and we need to go to the database more often than the set threshold value.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> IH aggregated data is not up to date</t>
+  </si>
+  <si>
+    <t>alerts/ihAggregationReadIHPercentage</t>
+  </si>
+  <si>
+    <t>PEGA0096</t>
+  </si>
+  <si>
+    <t>Raise an alert when the average read time for IH aggregated data is above the set threshold value.</t>
+  </si>
+  <si>
+    <t>Average read time for IH aggregated data is above the threshold value.</t>
+  </si>
+  <si>
+    <t>alerts/ihAggregationReadTimeThreshold</t>
+  </si>
+  <si>
+    <t>PEGA0097</t>
+  </si>
+  <si>
+    <t>Maximum active sessions limit reached</t>
+  </si>
+  <si>
+    <t>Raise an alert when maximum active sessions limit reached</t>
+  </si>
+  <si>
+    <t>cluster/requestors/browser/maxactive/block</t>
+  </si>
+  <si>
+    <t>BOOLEAN</t>
+  </si>
+  <si>
+    <t>https://pdn.pega.com/node/1392991</t>
+  </si>
+  <si>
+    <t>Number of servers in the cluster falls below the recommended settings</t>
+  </si>
+  <si>
+    <t>This alert is generated for Apache Ignite servers when the number of servers in the cluster falls below the recommended minimum. The recommended minimum number of server nodes deployed in the cluster is based on the failover strategies for distributed assets that are configured on the cluster. You need at least three Apache Ignite servers in a cluster. The alert is raised by all remaining operating nodes. If, after a first alert is sent, another server is removed from the cluster, a new alert is sent.</t>
+  </si>
+  <si>
+    <t>https://pdn.pega.com/node/1396436</t>
+  </si>
+  <si>
+    <t>This alert is generated for Apache Ignite servers when a client node (Pega® Platform node) has disconnected from the cluster. This alert occurs only when Pega Platform is configured as a client in an Apache Ignite client-server topology.</t>
+  </si>
+  <si>
+    <t>A node left the cluster</t>
+  </si>
+  <si>
+    <t>https://pdn.pega.com/node/1393796</t>
+  </si>
+  <si>
+    <t>This alert is generated for servers or clients in an Apache Ignite client-server topology when a node unexpectedly disconnects from the cluster and is considered failed.</t>
+  </si>
+  <si>
+    <t>Cluster segmentation causes subclusters to form</t>
+  </si>
+  <si>
+    <t>https://pdn.pega.com/node/1393791</t>
+  </si>
+  <si>
+    <t>This alert is generated for servers or clients in an Apache Ignite client-server topology when two or more subclusters are formed from cluster segmentation. Nodes in each subcluster do not see the nodes from the other subcluster and depending on how the subclusters were formed, the data might be lost.</t>
+  </si>
+  <si>
+    <t>Data stored in one or more cluster caches is lost</t>
+  </si>
+  <si>
+    <t>https://pdn.pega.com/node/1393741</t>
+  </si>
+  <si>
+    <t>This alert is generated for servers or clients in an Apache Ignite client-server topology when data that is stored in one or more cluster caches is lost. The data that can be lost is the distributed features data that is spread across the cluster among different nodes.</t>
   </si>
 </sst>
 </file>
@@ -1829,9 +1919,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1895,8 +1988,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:O106" tableType="xml" totalsRowShown="0" connectionId="1">
-  <autoFilter ref="A1:O106"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:O111" tableType="xml" totalsRowShown="0" connectionId="1">
+  <autoFilter ref="A1:O111"/>
   <tableColumns count="15">
     <tableColumn id="1" uniqueName="Id" name="Id">
       <xmlColumnPr mapId="1" xpath="/AlertMessageList/AlertMessage/Id" xmlDataType="int"/>
@@ -2211,10 +2304,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O106"/>
+  <dimension ref="A1:O111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C54" workbookViewId="0">
-      <selection activeCell="G87" sqref="G87"/>
+    <sheetView tabSelected="1" topLeftCell="I74" workbookViewId="0">
+      <selection activeCell="L92" sqref="L92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4118,7 +4211,7 @@
         <v>264</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
       <c r="I43" s="1" t="s">
         <v>433</v>
@@ -6065,16 +6158,16 @@
         <v>118</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
       <c r="F85" s="1" t="s">
         <v>221</v>
       </c>
       <c r="G85" s="1" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
       <c r="H85" s="1" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
       <c r="I85" s="1" t="s">
         <v>436</v>
@@ -6112,16 +6205,16 @@
         <v>118</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="F86" s="1" t="s">
         <v>221</v>
       </c>
       <c r="G86" s="1" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="H86" s="1" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
       <c r="I86" s="1"/>
       <c r="J86" s="1"/>
@@ -6153,10 +6246,10 @@
         <v>221</v>
       </c>
       <c r="G87" s="1" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="H87" s="1" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
       <c r="I87" s="1"/>
       <c r="J87" s="1"/>
@@ -6176,23 +6269,31 @@
         <v>572</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="F88" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="G88" s="1"/>
-      <c r="H88" s="1"/>
-      <c r="I88" s="1"/>
+      <c r="G88" s="1" t="s">
+        <v>608</v>
+      </c>
+      <c r="H88" s="1" t="s">
+        <v>609</v>
+      </c>
+      <c r="I88" s="1" t="s">
+        <v>419</v>
+      </c>
       <c r="J88" s="1"/>
       <c r="K88" s="1"/>
-      <c r="L88" s="1"/>
+      <c r="L88" s="1" t="s">
+        <v>496</v>
+      </c>
       <c r="M88" s="1"/>
       <c r="N88" s="1"/>
       <c r="O88" s="1" t="s">
@@ -6207,23 +6308,31 @@
         <v>573</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>576</v>
+        <v>610</v>
       </c>
       <c r="F89" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="G89" s="1"/>
-      <c r="H89" s="1"/>
-      <c r="I89" s="1"/>
+      <c r="G89" s="1" t="s">
+        <v>611</v>
+      </c>
+      <c r="H89" s="1" t="s">
+        <v>612</v>
+      </c>
+      <c r="I89" s="1" t="s">
+        <v>419</v>
+      </c>
       <c r="J89" s="1"/>
       <c r="K89" s="1"/>
-      <c r="L89" s="1"/>
+      <c r="L89" s="1" t="s">
+        <v>496</v>
+      </c>
       <c r="M89" s="1"/>
       <c r="N89" s="1"/>
       <c r="O89" s="1" t="s">
@@ -6238,23 +6347,31 @@
         <v>574</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>578</v>
+        <v>613</v>
       </c>
       <c r="F90" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="G90" s="1"/>
-      <c r="H90" s="1"/>
-      <c r="I90" s="1"/>
+      <c r="G90" s="1" t="s">
+        <v>614</v>
+      </c>
+      <c r="H90" s="1" t="s">
+        <v>615</v>
+      </c>
+      <c r="I90" s="1" t="s">
+        <v>419</v>
+      </c>
       <c r="J90" s="1"/>
       <c r="K90" s="1"/>
-      <c r="L90" s="1"/>
+      <c r="L90" s="1" t="s">
+        <v>496</v>
+      </c>
       <c r="M90" s="1"/>
       <c r="N90" s="1"/>
       <c r="O90" s="1" t="s">
@@ -6269,23 +6386,31 @@
         <v>575</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>579</v>
+        <v>616</v>
       </c>
       <c r="F91" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="G91" s="1"/>
-      <c r="H91" s="1"/>
-      <c r="I91" s="1"/>
+      <c r="G91" s="2" t="s">
+        <v>617</v>
+      </c>
+      <c r="H91" s="1" t="s">
+        <v>618</v>
+      </c>
+      <c r="I91" s="1" t="s">
+        <v>419</v>
+      </c>
       <c r="J91" s="1"/>
       <c r="K91" s="1"/>
-      <c r="L91" s="1"/>
+      <c r="L91" s="1" t="s">
+        <v>496</v>
+      </c>
       <c r="M91" s="1"/>
       <c r="N91" s="1"/>
       <c r="O91" s="1" t="s">
@@ -6294,66 +6419,76 @@
     </row>
     <row r="92" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A92">
-        <v>201</v>
+        <v>92</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>98</v>
+        <v>586</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>207</v>
+        <v>606</v>
       </c>
       <c r="F92" s="1" t="s">
         <v>221</v>
       </c>
       <c r="G92" s="1" t="s">
-        <v>303</v>
+        <v>605</v>
       </c>
       <c r="H92" s="1" t="s">
-        <v>399</v>
-      </c>
-      <c r="I92" s="1"/>
-      <c r="J92" s="1"/>
+        <v>607</v>
+      </c>
+      <c r="I92" s="1" t="s">
+        <v>590</v>
+      </c>
+      <c r="J92" s="1" t="s">
+        <v>439</v>
+      </c>
       <c r="K92" s="1"/>
-      <c r="L92" s="1"/>
-      <c r="M92" s="1"/>
-      <c r="N92" s="1"/>
+      <c r="L92" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="M92" s="1" t="s">
+        <v>501</v>
+      </c>
+      <c r="N92" s="1" t="s">
+        <v>591</v>
+      </c>
       <c r="O92" s="1" t="s">
         <v>557</v>
       </c>
     </row>
     <row r="93" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A93">
-        <v>202</v>
+        <v>93</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>99</v>
+        <v>587</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>208</v>
+        <v>588</v>
       </c>
       <c r="F93" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="G93" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="H93" s="1" t="s">
-        <v>400</v>
-      </c>
-      <c r="I93" s="1"/>
-      <c r="J93" s="1"/>
+      <c r="G93" s="1"/>
+      <c r="H93" s="1"/>
+      <c r="I93" s="1" t="s">
+        <v>589</v>
+      </c>
+      <c r="J93" s="1" t="s">
+        <v>439</v>
+      </c>
       <c r="K93" s="1"/>
       <c r="L93" s="1"/>
       <c r="M93" s="1"/>
@@ -6364,133 +6499,161 @@
     </row>
     <row r="94" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A94">
-        <v>203</v>
+        <v>94</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>100</v>
+        <v>592</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>209</v>
+        <v>594</v>
       </c>
       <c r="F94" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="G94" s="1" t="s">
-        <v>305</v>
-      </c>
+      <c r="G94" s="1"/>
       <c r="H94" s="1" t="s">
-        <v>401</v>
-      </c>
-      <c r="I94" s="1"/>
-      <c r="J94" s="1"/>
-      <c r="K94" s="1"/>
-      <c r="L94" s="1"/>
-      <c r="M94" s="1"/>
-      <c r="N94" s="1"/>
+        <v>593</v>
+      </c>
+      <c r="I94" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="J94" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="K94" s="1" t="s">
+        <v>595</v>
+      </c>
+      <c r="L94" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="M94" s="1" t="s">
+        <v>503</v>
+      </c>
+      <c r="N94" s="1" t="s">
+        <v>513</v>
+      </c>
       <c r="O94" s="1" t="s">
         <v>565</v>
       </c>
     </row>
     <row r="95" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A95">
-        <v>204</v>
+        <v>95</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>101</v>
+        <v>596</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>210</v>
+        <v>598</v>
       </c>
       <c r="F95" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="G95" s="1" t="s">
-        <v>306</v>
-      </c>
+      <c r="G95" s="1"/>
       <c r="H95" s="1" t="s">
-        <v>402</v>
-      </c>
-      <c r="I95" s="1"/>
-      <c r="J95" s="1"/>
-      <c r="K95" s="1"/>
-      <c r="L95" s="1"/>
-      <c r="M95" s="1"/>
-      <c r="N95" s="1"/>
+        <v>597</v>
+      </c>
+      <c r="I95" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="J95" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="K95" s="1" t="s">
+        <v>599</v>
+      </c>
+      <c r="L95" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="M95" s="1" t="s">
+        <v>499</v>
+      </c>
+      <c r="N95" s="1" t="s">
+        <v>513</v>
+      </c>
       <c r="O95" s="1" t="s">
         <v>542</v>
       </c>
     </row>
     <row r="96" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A96">
-        <v>205</v>
+        <v>96</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>102</v>
+        <v>600</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>211</v>
+        <v>601</v>
       </c>
       <c r="F96" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="G96" s="1" t="s">
-        <v>307</v>
-      </c>
+      <c r="G96" s="1"/>
       <c r="H96" s="1" t="s">
-        <v>403</v>
+        <v>602</v>
       </c>
       <c r="I96" s="1"/>
-      <c r="J96" s="1"/>
-      <c r="K96" s="1"/>
-      <c r="L96" s="1"/>
-      <c r="M96" s="1"/>
-      <c r="N96" s="1"/>
+      <c r="J96" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="K96" s="1" t="s">
+        <v>603</v>
+      </c>
+      <c r="L96" s="1" t="s">
+        <v>496</v>
+      </c>
+      <c r="M96" s="1" t="s">
+        <v>604</v>
+      </c>
+      <c r="N96" s="1" t="s">
+        <v>440</v>
+      </c>
       <c r="O96" s="1" t="s">
         <v>564</v>
       </c>
     </row>
     <row r="97" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A97">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="F97" s="1" t="s">
         <v>221</v>
       </c>
       <c r="G97" s="1" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="H97" s="1" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
       <c r="I97" s="1"/>
       <c r="J97" s="1"/>
@@ -6499,33 +6662,33 @@
       <c r="M97" s="1"/>
       <c r="N97" s="1"/>
       <c r="O97" s="1" t="s">
-        <v>543</v>
+        <v>557</v>
       </c>
     </row>
     <row r="98" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A98">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="F98" s="1" t="s">
         <v>221</v>
       </c>
       <c r="G98" s="1" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="H98" s="1" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
       <c r="I98" s="1"/>
       <c r="J98" s="1"/>
@@ -6534,33 +6697,33 @@
       <c r="M98" s="1"/>
       <c r="N98" s="1"/>
       <c r="O98" s="1" t="s">
-        <v>545</v>
+        <v>559</v>
       </c>
     </row>
     <row r="99" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A99">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="F99" s="1" t="s">
         <v>221</v>
       </c>
       <c r="G99" s="1" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="H99" s="1" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
       <c r="I99" s="1"/>
       <c r="J99" s="1"/>
@@ -6569,33 +6732,33 @@
       <c r="M99" s="1"/>
       <c r="N99" s="1"/>
       <c r="O99" s="1" t="s">
-        <v>546</v>
+        <v>565</v>
       </c>
     </row>
     <row r="100" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A100">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="F100" s="1" t="s">
         <v>221</v>
       </c>
       <c r="G100" s="1" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="H100" s="1" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
       <c r="I100" s="1"/>
       <c r="J100" s="1"/>
@@ -6604,15 +6767,15 @@
       <c r="M100" s="1"/>
       <c r="N100" s="1"/>
       <c r="O100" s="1" t="s">
-        <v>547</v>
+        <v>542</v>
       </c>
     </row>
     <row r="101" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A101">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="C101" s="1" t="s">
         <v>116</v>
@@ -6621,16 +6784,16 @@
         <v>123</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="F101" s="1" t="s">
         <v>221</v>
       </c>
       <c r="G101" s="1" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="H101" s="1" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="I101" s="1"/>
       <c r="J101" s="1"/>
@@ -6639,15 +6802,15 @@
       <c r="M101" s="1"/>
       <c r="N101" s="1"/>
       <c r="O101" s="1" t="s">
-        <v>557</v>
+        <v>564</v>
       </c>
     </row>
     <row r="102" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A102">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="C102" s="1" t="s">
         <v>116</v>
@@ -6656,16 +6819,16 @@
         <v>123</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="F102" s="1" t="s">
         <v>221</v>
       </c>
       <c r="G102" s="1" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="H102" s="1" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
       <c r="I102" s="1"/>
       <c r="J102" s="1"/>
@@ -6674,15 +6837,15 @@
       <c r="M102" s="1"/>
       <c r="N102" s="1"/>
       <c r="O102" s="1" t="s">
-        <v>559</v>
+        <v>543</v>
       </c>
     </row>
     <row r="103" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A103">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="C103" s="1" t="s">
         <v>116</v>
@@ -6691,16 +6854,16 @@
         <v>123</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="F103" s="1" t="s">
         <v>221</v>
       </c>
       <c r="G103" s="1" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="H103" s="1" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="I103" s="1"/>
       <c r="J103" s="1"/>
@@ -6709,15 +6872,15 @@
       <c r="M103" s="1"/>
       <c r="N103" s="1"/>
       <c r="O103" s="1" t="s">
-        <v>565</v>
+        <v>545</v>
       </c>
     </row>
     <row r="104" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A104">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="C104" s="1" t="s">
         <v>116</v>
@@ -6726,16 +6889,16 @@
         <v>123</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="F104" s="1" t="s">
         <v>221</v>
       </c>
       <c r="G104" s="1" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="H104" s="1" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="I104" s="1"/>
       <c r="J104" s="1"/>
@@ -6744,15 +6907,15 @@
       <c r="M104" s="1"/>
       <c r="N104" s="1"/>
       <c r="O104" s="1" t="s">
-        <v>542</v>
+        <v>546</v>
       </c>
     </row>
     <row r="105" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A105">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="C105" s="1" t="s">
         <v>116</v>
@@ -6761,16 +6924,16 @@
         <v>123</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="F105" s="1" t="s">
         <v>221</v>
       </c>
       <c r="G105" s="1" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="H105" s="1" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
       <c r="I105" s="1"/>
       <c r="J105" s="1"/>
@@ -6779,33 +6942,33 @@
       <c r="M105" s="1"/>
       <c r="N105" s="1"/>
       <c r="O105" s="1" t="s">
-        <v>564</v>
+        <v>547</v>
       </c>
     </row>
     <row r="106" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A106">
-        <v>301</v>
+        <v>210</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>117</v>
+        <v>216</v>
       </c>
       <c r="F106" s="1" t="s">
         <v>221</v>
       </c>
       <c r="G106" s="1" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="H106" s="1" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
       <c r="I106" s="1"/>
       <c r="J106" s="1"/>
@@ -6814,13 +6977,192 @@
       <c r="M106" s="1"/>
       <c r="N106" s="1"/>
       <c r="O106" s="1" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="107" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A107">
+        <v>211</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D107" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E107" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="F107" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="G107" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="H107" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="I107" s="1"/>
+      <c r="J107" s="1"/>
+      <c r="K107" s="1"/>
+      <c r="L107" s="1"/>
+      <c r="M107" s="1"/>
+      <c r="N107" s="1"/>
+      <c r="O107" s="1" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="108" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A108">
+        <v>212</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D108" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E108" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="F108" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="G108" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="H108" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="I108" s="1"/>
+      <c r="J108" s="1"/>
+      <c r="K108" s="1"/>
+      <c r="L108" s="1"/>
+      <c r="M108" s="1"/>
+      <c r="N108" s="1"/>
+      <c r="O108" s="1" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="109" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A109">
+        <v>213</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D109" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E109" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="F109" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="G109" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="H109" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="I109" s="1"/>
+      <c r="J109" s="1"/>
+      <c r="K109" s="1"/>
+      <c r="L109" s="1"/>
+      <c r="M109" s="1"/>
+      <c r="N109" s="1"/>
+      <c r="O109" s="1" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="110" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A110">
+        <v>214</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D110" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E110" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="F110" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="G110" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="H110" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="I110" s="1"/>
+      <c r="J110" s="1"/>
+      <c r="K110" s="1"/>
+      <c r="L110" s="1"/>
+      <c r="M110" s="1"/>
+      <c r="N110" s="1"/>
+      <c r="O110" s="1" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="111" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A111">
+        <v>301</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D111" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E111" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F111" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="G111" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="H111" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="I111" s="1"/>
+      <c r="J111" s="1"/>
+      <c r="K111" s="1"/>
+      <c r="L111" s="1"/>
+      <c r="M111" s="1"/>
+      <c r="N111" s="1"/>
+      <c r="O111" s="1" t="s">
         <v>560</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G87" r:id="rId1"/>
+    <hyperlink ref="G92" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Support for newer CloudK logs Fixed checkstyle and errorprone warnings
</commit_message>
<xml_diff>
--- a/src/main/resources/AlertMessageList.xlsx
+++ b/src/main/resources/AlertMessageList.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_PRIVATE\Github_Master\pega-logviewer\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C8852FB-8FDB-465E-9B8C-893D6D960EB1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2580C9B5-18A9-475F-9D4E-450195B1287B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{10474AC9-EC98-4A01-86DB-DE0ABEBDFAED}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1955" uniqueCount="923">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2027" uniqueCount="961">
   <si>
     <t>Id</t>
   </si>
@@ -2797,6 +2797,120 @@
   </si>
   <si>
     <t>512</t>
+  </si>
+  <si>
+    <t>https://docs.pega.com/pega0135-local-file-path-used-source-location-cloud-system</t>
+  </si>
+  <si>
+    <t>On a Pega Cloud® system, using a local file path in the source location for a file listener is an incorrect configuration</t>
+  </si>
+  <si>
+    <t>https://docs.pega.com/pega0136-goofys-enabled-path-used-source-location-cloud-system</t>
+  </si>
+  <si>
+    <t>On a Pega Cloud® system, using a Goofys-enabled path in the source location is not a recommended practice</t>
+  </si>
+  <si>
+    <t>https://docs.pega.com/pega0138-alert-simulation-run-simid-not-fully-optimized</t>
+  </si>
+  <si>
+    <t>Triggers the PEGA0138 alert when a simulation test that you run in the Business Operations Environment (BOE) of your Pega Customer Decision Hub™ system is not optimized because the strategy components include configuration patterns that are incompatible with optimization</t>
+  </si>
+  <si>
+    <t>https://docs.pega.com/pega0139-email-account-throttled</t>
+  </si>
+  <si>
+    <t>This alert indicates that an email provider is throttling one of your email accounts.</t>
+  </si>
+  <si>
+    <t>https://docs.pega.com/pega0140-listener-failed-process-email-last-recovery-attempt</t>
+  </si>
+  <si>
+    <t>The number of times that the email listener attempts to process an email, before the listener logs an error message.</t>
+  </si>
+  <si>
+    <t>Generates this alert when the email listener attempts to delete multiple email messages from the Inbox and move them to the Deleted items folder, but that folder is full</t>
+  </si>
+  <si>
+    <t>https://docs.pega.com/pega0141-email-expunge-failed-during-message-post-processing</t>
+  </si>
+  <si>
+    <t>https://docs.pega.com/pega0142-email-status-not-updated-more-two-hours</t>
+  </si>
+  <si>
+    <t>This alert indicates that multiple email messages exceeded the processing time threshold.</t>
+  </si>
+  <si>
+    <t>https://docs.pega.com/pega0143-log-service-email-errors-exceed-record-limit</t>
+  </si>
+  <si>
+    <t>This alert indicates a critical issue in which multiple failures to process email messages might have a significant business impact.</t>
+  </si>
+  <si>
+    <t>PEGA0144</t>
+  </si>
+  <si>
+    <t>PEGA0145</t>
+  </si>
+  <si>
+    <t>PEGA0146</t>
+  </si>
+  <si>
+    <t>PEGA0147</t>
+  </si>
+  <si>
+    <t>Email Listener</t>
+  </si>
+  <si>
+    <t>Simulations</t>
+  </si>
+  <si>
+    <t>File Listener</t>
+  </si>
+  <si>
+    <t>Stability</t>
+  </si>
+  <si>
+    <t>Tracer file size</t>
+  </si>
+  <si>
+    <t>Remote case types time-out</t>
+  </si>
+  <si>
+    <t>Local file path used as source location on a cloud system</t>
+  </si>
+  <si>
+    <t>Goofys-enabled path used as source location on a cloud system</t>
+  </si>
+  <si>
+    <t>Simulation run [SimID] not fully optimized</t>
+  </si>
+  <si>
+    <t>Email account is throttled</t>
+  </si>
+  <si>
+    <t>Listener failed to process an email in the last recovery attempt</t>
+  </si>
+  <si>
+    <t>Email expunge failed during message post-processing</t>
+  </si>
+  <si>
+    <t>Email status not updated for more than two hours</t>
+  </si>
+  <si>
+    <t>Log-Service-Email errors exceed the record limit</t>
+  </si>
+  <si>
+    <t>https://docs.pega.com/pega0132-alert-time-out-threshold-exceeded-remote-case-type-requests</t>
+  </si>
+  <si>
+    <t>https://docs.pega.com/secu0021-alert-expired-certificate</t>
+  </si>
+  <si>
+    <t>Expired Certificate</t>
+  </si>
+  <si>
+    <t>The system generates security alert SECU0021 when an attempt has been made to import an expired certificate into the platform truststore.</t>
   </si>
 </sst>
 </file>
@@ -2954,8 +3068,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{179863B1-6A76-4246-A1BC-FE8FC898012F}" name="Table1" displayName="Table1" ref="A1:O165" tableType="xml" totalsRowShown="0" connectionId="1">
-  <autoFilter ref="A1:O165" xr:uid="{4F6276EB-680B-458A-B167-A8C1331B3E93}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{179863B1-6A76-4246-A1BC-FE8FC898012F}" name="Table1" displayName="Table1" ref="A1:O169" tableType="xml" totalsRowShown="0" connectionId="1">
+  <autoFilter ref="A1:O169" xr:uid="{4F6276EB-680B-458A-B167-A8C1331B3E93}"/>
   <tableColumns count="15">
     <tableColumn id="1" xr3:uid="{39609868-3AA4-445A-A488-970B25180B73}" uniqueName="Id" name="Id">
       <xmlColumnPr mapId="1" xpath="/AlertMessageList/AlertMessage/Id" xmlDataType="int"/>
@@ -3304,34 +3418,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O165"/>
+  <dimension ref="A1:O169"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A93" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A127" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A82" sqref="A82"/>
-      <selection pane="topRight" activeCell="H110" sqref="H110"/>
+      <selection pane="topRight" activeCell="A173" sqref="A173"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" customWidth="1"/>
-    <col min="5" max="5" width="60.42578125" customWidth="1"/>
-    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="100.140625" customWidth="1"/>
-    <col min="8" max="8" width="141.7109375" customWidth="1"/>
-    <col min="9" max="9" width="48.85546875" customWidth="1"/>
-    <col min="10" max="10" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="61.28515625" customWidth="1"/>
-    <col min="12" max="12" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="60.453125" customWidth="1"/>
+    <col min="6" max="6" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="100.1796875" customWidth="1"/>
+    <col min="8" max="8" width="141.7265625" customWidth="1"/>
+    <col min="9" max="9" width="48.81640625" customWidth="1"/>
+    <col min="10" max="10" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="61.26953125" customWidth="1"/>
+    <col min="12" max="12" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="24.54296875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="49" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3378,7 +3492,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3425,7 +3539,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3472,7 +3586,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3519,7 +3633,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -3566,7 +3680,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -3613,7 +3727,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -3652,7 +3766,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -3691,7 +3805,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -3730,7 +3844,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -3769,7 +3883,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -3808,7 +3922,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -3855,7 +3969,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
@@ -3894,7 +4008,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
@@ -3933,7 +4047,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
@@ -3972,7 +4086,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
@@ -4011,7 +4125,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
@@ -4056,7 +4170,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
@@ -4101,7 +4215,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>18</v>
       </c>
@@ -4148,7 +4262,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>19</v>
       </c>
@@ -4195,7 +4309,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>20</v>
       </c>
@@ -4242,7 +4356,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>21</v>
       </c>
@@ -4289,7 +4403,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>22</v>
       </c>
@@ -4334,7 +4448,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>23</v>
       </c>
@@ -4379,7 +4493,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>24</v>
       </c>
@@ -4426,7 +4540,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>25</v>
       </c>
@@ -4473,7 +4587,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>26</v>
       </c>
@@ -4518,7 +4632,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>27</v>
       </c>
@@ -4563,7 +4677,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>28</v>
       </c>
@@ -4598,7 +4712,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>29</v>
       </c>
@@ -4645,7 +4759,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>30</v>
       </c>
@@ -4692,7 +4806,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>31</v>
       </c>
@@ -4727,7 +4841,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>32</v>
       </c>
@@ -4774,7 +4888,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>33</v>
       </c>
@@ -4821,7 +4935,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>34</v>
       </c>
@@ -4868,7 +4982,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>35</v>
       </c>
@@ -4915,7 +5029,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>36</v>
       </c>
@@ -4956,7 +5070,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>37</v>
       </c>
@@ -5003,7 +5117,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>38</v>
       </c>
@@ -5050,7 +5164,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>39</v>
       </c>
@@ -5097,7 +5211,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>40</v>
       </c>
@@ -5144,7 +5258,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>41</v>
       </c>
@@ -5191,7 +5305,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>42</v>
       </c>
@@ -5238,7 +5352,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>43</v>
       </c>
@@ -5285,7 +5399,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>44</v>
       </c>
@@ -5332,7 +5446,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>45</v>
       </c>
@@ -5379,7 +5493,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>46</v>
       </c>
@@ -5426,7 +5540,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>47</v>
       </c>
@@ -5473,7 +5587,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>48</v>
       </c>
@@ -5520,7 +5634,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>49</v>
       </c>
@@ -5567,7 +5681,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>50</v>
       </c>
@@ -5614,7 +5728,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>51</v>
       </c>
@@ -5657,7 +5771,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>52</v>
       </c>
@@ -5704,7 +5818,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>53</v>
       </c>
@@ -5751,7 +5865,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>54</v>
       </c>
@@ -5798,7 +5912,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>55</v>
       </c>
@@ -5845,7 +5959,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>56</v>
       </c>
@@ -5892,7 +6006,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>58</v>
       </c>
@@ -5939,7 +6053,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>59</v>
       </c>
@@ -5986,7 +6100,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>60</v>
       </c>
@@ -6033,7 +6147,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>61</v>
       </c>
@@ -6080,7 +6194,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>62</v>
       </c>
@@ -6127,7 +6241,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>63</v>
       </c>
@@ -6174,7 +6288,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>64</v>
       </c>
@@ -6221,7 +6335,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>65</v>
       </c>
@@ -6268,7 +6382,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>66</v>
       </c>
@@ -6311,7 +6425,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>67</v>
       </c>
@@ -6358,7 +6472,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>68</v>
       </c>
@@ -6405,7 +6519,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>69</v>
       </c>
@@ -6452,7 +6566,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A70">
         <v>70</v>
       </c>
@@ -6499,7 +6613,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>71</v>
       </c>
@@ -6546,7 +6660,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A72">
         <v>72</v>
       </c>
@@ -6593,7 +6707,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A73">
         <v>73</v>
       </c>
@@ -6640,7 +6754,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A74">
         <v>74</v>
       </c>
@@ -6687,7 +6801,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A75">
         <v>75</v>
       </c>
@@ -6734,7 +6848,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A76">
         <v>76</v>
       </c>
@@ -6781,7 +6895,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A77">
         <v>77</v>
       </c>
@@ -6828,7 +6942,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A78">
         <v>78</v>
       </c>
@@ -6875,7 +6989,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A79">
         <v>79</v>
       </c>
@@ -6922,7 +7036,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A80">
         <v>80</v>
       </c>
@@ -6969,7 +7083,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="81" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A81">
         <v>81</v>
       </c>
@@ -7016,7 +7130,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="82" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A82">
         <v>82</v>
       </c>
@@ -7026,6 +7140,9 @@
       <c r="C82" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="D82" t="s">
+        <v>634</v>
+      </c>
       <c r="E82" t="s">
         <v>634</v>
       </c>
@@ -7060,7 +7177,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="83" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A83">
         <v>83</v>
       </c>
@@ -7070,6 +7187,9 @@
       <c r="C83" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="D83" t="s">
+        <v>635</v>
+      </c>
       <c r="E83" t="s">
         <v>635</v>
       </c>
@@ -7104,7 +7224,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="84" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A84">
         <v>84</v>
       </c>
@@ -7149,7 +7269,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="85" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A85">
         <v>85</v>
       </c>
@@ -7196,7 +7316,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="86" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A86">
         <v>86</v>
       </c>
@@ -7243,7 +7363,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="87" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A87">
         <v>87</v>
       </c>
@@ -7290,7 +7410,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="88" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A88">
         <v>88</v>
       </c>
@@ -7329,7 +7449,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="89" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A89">
         <v>89</v>
       </c>
@@ -7368,7 +7488,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="90" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A90">
         <v>90</v>
       </c>
@@ -7407,7 +7527,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="91" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A91">
         <v>91</v>
       </c>
@@ -7446,7 +7566,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="92" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A92">
         <v>92</v>
       </c>
@@ -7493,7 +7613,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="93" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A93">
         <v>93</v>
       </c>
@@ -7540,7 +7660,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="94" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A94">
         <v>94</v>
       </c>
@@ -7583,7 +7703,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="95" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A95">
         <v>95</v>
       </c>
@@ -7628,7 +7748,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="96" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A96">
         <v>96</v>
       </c>
@@ -7673,7 +7793,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="97" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A97">
         <v>97</v>
       </c>
@@ -7720,7 +7840,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="98" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A98">
         <v>98</v>
       </c>
@@ -7759,7 +7879,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="99" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A99">
         <v>99</v>
       </c>
@@ -7798,7 +7918,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="100" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A100">
         <v>100</v>
       </c>
@@ -7837,7 +7957,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="101" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A101">
         <v>101</v>
       </c>
@@ -7876,7 +7996,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="102" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A102">
         <v>102</v>
       </c>
@@ -7915,7 +8035,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="103" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A103">
         <v>103</v>
       </c>
@@ -7954,7 +8074,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="104" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A104">
         <v>104</v>
       </c>
@@ -7993,7 +8113,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="105" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A105">
         <v>105</v>
       </c>
@@ -8040,7 +8160,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="106" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A106">
         <v>106</v>
       </c>
@@ -8079,7 +8199,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="107" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A107">
         <v>107</v>
       </c>
@@ -8126,7 +8246,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="108" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A108">
         <v>108</v>
       </c>
@@ -8163,7 +8283,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="109" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A109">
         <v>109</v>
       </c>
@@ -8210,7 +8330,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="110" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A110">
         <v>110</v>
       </c>
@@ -8257,7 +8377,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="111" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A111">
         <v>111</v>
       </c>
@@ -8298,7 +8418,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="112" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A112">
         <v>112</v>
       </c>
@@ -8339,7 +8459,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="113" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A113">
         <v>113</v>
       </c>
@@ -8380,7 +8500,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="114" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A114">
         <v>114</v>
       </c>
@@ -8421,7 +8541,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="115" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A115">
         <v>115</v>
       </c>
@@ -8462,7 +8582,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="116" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A116">
         <v>116</v>
       </c>
@@ -8503,7 +8623,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="117" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A117">
         <v>117</v>
       </c>
@@ -8544,7 +8664,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="118" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A118">
         <v>118</v>
       </c>
@@ -8585,7 +8705,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="119" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A119">
         <v>119</v>
       </c>
@@ -8632,7 +8752,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="120" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A120">
         <v>120</v>
       </c>
@@ -8675,7 +8795,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="121" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A121">
         <v>121</v>
       </c>
@@ -8716,7 +8836,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="122" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A122">
         <v>122</v>
       </c>
@@ -8753,7 +8873,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="123" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A123">
         <v>123</v>
       </c>
@@ -8790,7 +8910,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="124" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A124">
         <v>124</v>
       </c>
@@ -8827,7 +8947,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="125" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A125">
         <v>125</v>
       </c>
@@ -8838,7 +8958,7 @@
         <v>17</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>108</v>
+        <v>946</v>
       </c>
       <c r="E125" s="1" t="s">
         <v>815</v>
@@ -8866,7 +8986,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="126" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A126">
         <v>126</v>
       </c>
@@ -8877,7 +8997,7 @@
         <v>17</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>108</v>
+        <v>946</v>
       </c>
       <c r="E126" s="1" t="s">
         <v>819</v>
@@ -8905,7 +9025,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="127" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A127">
         <v>127</v>
       </c>
@@ -8916,7 +9036,7 @@
         <v>17</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>108</v>
+        <v>946</v>
       </c>
       <c r="E127" s="1" t="s">
         <v>822</v>
@@ -8944,7 +9064,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="128" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A128">
         <v>128</v>
       </c>
@@ -8983,7 +9103,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="129" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A129">
         <v>129</v>
       </c>
@@ -8994,7 +9114,7 @@
         <v>17</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>108</v>
+        <v>947</v>
       </c>
       <c r="E129" s="1" t="s">
         <v>841</v>
@@ -9030,7 +9150,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="130" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A130">
         <v>130</v>
       </c>
@@ -9041,7 +9161,7 @@
         <v>17</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>108</v>
+        <v>663</v>
       </c>
       <c r="E130" s="1" t="s">
         <v>846</v>
@@ -9077,7 +9197,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="131" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A131">
         <v>131</v>
       </c>
@@ -9088,7 +9208,7 @@
         <v>17</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>108</v>
+        <v>946</v>
       </c>
       <c r="E131" s="1" t="s">
         <v>852</v>
@@ -9116,7 +9236,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="132" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A132">
         <v>132</v>
       </c>
@@ -9127,7 +9247,7 @@
         <v>17</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>108</v>
+        <v>948</v>
       </c>
       <c r="E132" s="1" t="s">
         <v>853</v>
@@ -9135,7 +9255,9 @@
       <c r="F132" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G132" s="1"/>
+      <c r="G132" s="1" t="s">
+        <v>957</v>
+      </c>
       <c r="H132" s="1" t="s">
         <v>854</v>
       </c>
@@ -9153,7 +9275,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="133" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A133">
         <v>133</v>
       </c>
@@ -9164,7 +9286,7 @@
         <v>17</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>108</v>
+        <v>576</v>
       </c>
       <c r="E133" s="1" t="s">
         <v>856</v>
@@ -9192,7 +9314,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="134" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A134">
         <v>134</v>
       </c>
@@ -9203,7 +9325,7 @@
         <v>17</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>108</v>
+        <v>641</v>
       </c>
       <c r="E134" s="1" t="s">
         <v>859</v>
@@ -9233,7 +9355,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="135" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A135">
         <v>135</v>
       </c>
@@ -9244,18 +9366,26 @@
         <v>17</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="E135" s="1"/>
+        <v>945</v>
+      </c>
+      <c r="E135" s="1" t="s">
+        <v>949</v>
+      </c>
       <c r="F135" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G135" s="1"/>
-      <c r="H135" s="1"/>
+      <c r="G135" s="1" t="s">
+        <v>923</v>
+      </c>
+      <c r="H135" s="1" t="s">
+        <v>924</v>
+      </c>
       <c r="I135" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="J135" s="1"/>
+      <c r="J135" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="K135" s="1"/>
       <c r="L135" s="1" t="s">
         <v>73</v>
@@ -9266,7 +9396,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="136" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A136">
         <v>136</v>
       </c>
@@ -9277,18 +9407,26 @@
         <v>17</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="E136" s="1"/>
+        <v>945</v>
+      </c>
+      <c r="E136" s="1" t="s">
+        <v>950</v>
+      </c>
       <c r="F136" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G136" s="1"/>
-      <c r="H136" s="1"/>
+      <c r="G136" s="1" t="s">
+        <v>925</v>
+      </c>
+      <c r="H136" s="1" t="s">
+        <v>926</v>
+      </c>
       <c r="I136" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="J136" s="1"/>
+      <c r="J136" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="K136" s="1"/>
       <c r="L136" s="1" t="s">
         <v>73</v>
@@ -9299,7 +9437,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="137" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A137">
         <v>137</v>
       </c>
@@ -9310,7 +9448,7 @@
         <v>17</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>108</v>
+        <v>641</v>
       </c>
       <c r="E137" s="1" t="s">
         <v>863</v>
@@ -9342,7 +9480,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="138" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A138">
         <v>138</v>
       </c>
@@ -9353,18 +9491,26 @@
         <v>17</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="E138" s="1"/>
+        <v>944</v>
+      </c>
+      <c r="E138" s="1" t="s">
+        <v>951</v>
+      </c>
       <c r="F138" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G138" s="1"/>
-      <c r="H138" s="1"/>
+      <c r="G138" s="1" t="s">
+        <v>927</v>
+      </c>
+      <c r="H138" s="1" t="s">
+        <v>928</v>
+      </c>
       <c r="I138" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="J138" s="1"/>
+      <c r="J138" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="K138" s="1"/>
       <c r="L138" s="1" t="s">
         <v>73</v>
@@ -9375,7 +9521,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="139" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A139">
         <v>139</v>
       </c>
@@ -9386,18 +9532,26 @@
         <v>17</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="E139" s="1"/>
+        <v>943</v>
+      </c>
+      <c r="E139" s="1" t="s">
+        <v>952</v>
+      </c>
       <c r="F139" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G139" s="1"/>
-      <c r="H139" s="1"/>
+      <c r="G139" s="1" t="s">
+        <v>929</v>
+      </c>
+      <c r="H139" s="1" t="s">
+        <v>930</v>
+      </c>
       <c r="I139" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="J139" s="1"/>
+      <c r="J139" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="K139" s="1"/>
       <c r="L139" s="1" t="s">
         <v>73</v>
@@ -9408,7 +9562,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="140" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A140">
         <v>140</v>
       </c>
@@ -9419,18 +9573,26 @@
         <v>17</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="E140" s="1"/>
+        <v>943</v>
+      </c>
+      <c r="E140" s="1" t="s">
+        <v>953</v>
+      </c>
       <c r="F140" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G140" s="1"/>
-      <c r="H140" s="1"/>
+      <c r="G140" s="1" t="s">
+        <v>931</v>
+      </c>
+      <c r="H140" s="1" t="s">
+        <v>932</v>
+      </c>
       <c r="I140" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="J140" s="1"/>
+      <c r="J140" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="K140" s="1"/>
       <c r="L140" s="1" t="s">
         <v>73</v>
@@ -9441,7 +9603,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="141" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A141">
         <v>141</v>
       </c>
@@ -9452,18 +9614,26 @@
         <v>17</v>
       </c>
       <c r="D141" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="E141" s="1"/>
+        <v>943</v>
+      </c>
+      <c r="E141" s="1" t="s">
+        <v>954</v>
+      </c>
       <c r="F141" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G141" s="1"/>
-      <c r="H141" s="1"/>
+      <c r="G141" s="1" t="s">
+        <v>934</v>
+      </c>
+      <c r="H141" s="1" t="s">
+        <v>933</v>
+      </c>
       <c r="I141" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="J141" s="1"/>
+      <c r="J141" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="K141" s="1"/>
       <c r="L141" s="1" t="s">
         <v>73</v>
@@ -9474,7 +9644,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="142" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A142">
         <v>142</v>
       </c>
@@ -9485,18 +9655,26 @@
         <v>17</v>
       </c>
       <c r="D142" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="E142" s="1"/>
+        <v>943</v>
+      </c>
+      <c r="E142" s="1" t="s">
+        <v>955</v>
+      </c>
       <c r="F142" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G142" s="1"/>
-      <c r="H142" s="1"/>
+      <c r="G142" s="1" t="s">
+        <v>935</v>
+      </c>
+      <c r="H142" s="1" t="s">
+        <v>936</v>
+      </c>
       <c r="I142" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="J142" s="1"/>
+      <c r="J142" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="K142" s="1"/>
       <c r="L142" s="1" t="s">
         <v>73</v>
@@ -9507,7 +9685,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="143" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A143">
         <v>143</v>
       </c>
@@ -9518,18 +9696,26 @@
         <v>17</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="E143" s="1"/>
+        <v>943</v>
+      </c>
+      <c r="E143" s="1" t="s">
+        <v>956</v>
+      </c>
       <c r="F143" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G143" s="1"/>
-      <c r="H143" s="1"/>
+      <c r="G143" s="1" t="s">
+        <v>937</v>
+      </c>
+      <c r="H143" s="1" t="s">
+        <v>938</v>
+      </c>
       <c r="I143" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="J143" s="1"/>
+      <c r="J143" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="K143" s="1"/>
       <c r="L143" s="1" t="s">
         <v>73</v>
@@ -9540,31 +9726,25 @@
         <v>119</v>
       </c>
     </row>
-    <row r="144" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A144">
-        <v>201</v>
+        <v>144</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>470</v>
+        <v>939</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>471</v>
+        <v>17</v>
       </c>
       <c r="D144" s="1" t="s">
-        <v>472</v>
-      </c>
-      <c r="E144" t="s">
-        <v>473</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="E144" s="1"/>
       <c r="F144" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G144" t="s">
-        <v>865</v>
-      </c>
-      <c r="H144" s="1" t="s">
-        <v>474</v>
-      </c>
+      <c r="G144" s="1"/>
+      <c r="H144" s="1"/>
       <c r="I144" s="1" t="s">
         <v>72</v>
       </c>
@@ -9579,31 +9759,25 @@
         <v>123</v>
       </c>
     </row>
-    <row r="145" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A145">
-        <v>202</v>
+        <v>145</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>475</v>
+        <v>940</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>471</v>
+        <v>17</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>472</v>
-      </c>
-      <c r="E145" t="s">
-        <v>476</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="E145" s="1"/>
       <c r="F145" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G145" t="s">
-        <v>866</v>
-      </c>
-      <c r="H145" s="1" t="s">
-        <v>477</v>
-      </c>
+      <c r="G145" s="1"/>
+      <c r="H145" s="1"/>
       <c r="I145" s="1" t="s">
         <v>72</v>
       </c>
@@ -9615,34 +9789,28 @@
       <c r="M145" s="1"/>
       <c r="N145" s="1"/>
       <c r="O145" s="1" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="146" spans="1:15" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="146" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A146">
-        <v>203</v>
+        <v>146</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>478</v>
+        <v>941</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>471</v>
+        <v>17</v>
       </c>
       <c r="D146" s="1" t="s">
-        <v>472</v>
-      </c>
-      <c r="E146" t="s">
-        <v>479</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="E146" s="1"/>
       <c r="F146" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G146" t="s">
-        <v>867</v>
-      </c>
-      <c r="H146" s="1" t="s">
-        <v>480</v>
-      </c>
+      <c r="G146" s="1"/>
+      <c r="H146" s="1"/>
       <c r="I146" s="1" t="s">
         <v>72</v>
       </c>
@@ -9657,31 +9825,25 @@
         <v>138</v>
       </c>
     </row>
-    <row r="147" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A147">
-        <v>204</v>
+        <v>147</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>481</v>
+        <v>942</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>471</v>
+        <v>17</v>
       </c>
       <c r="D147" s="1" t="s">
-        <v>472</v>
-      </c>
-      <c r="E147" t="s">
-        <v>482</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="E147" s="1"/>
       <c r="F147" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G147" t="s">
-        <v>868</v>
-      </c>
-      <c r="H147" s="1" t="s">
-        <v>483</v>
-      </c>
+      <c r="G147" s="1"/>
+      <c r="H147" s="1"/>
       <c r="I147" s="1" t="s">
         <v>72</v>
       </c>
@@ -9693,33 +9855,33 @@
       <c r="M147" s="1"/>
       <c r="N147" s="1"/>
       <c r="O147" s="1" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="148" spans="1:15" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="148" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A148">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>484</v>
+        <v>470</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>485</v>
+        <v>471</v>
       </c>
       <c r="D148" s="1" t="s">
-        <v>486</v>
+        <v>472</v>
       </c>
       <c r="E148" t="s">
-        <v>487</v>
+        <v>473</v>
       </c>
       <c r="F148" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G148" t="s">
-        <v>869</v>
+        <v>865</v>
       </c>
       <c r="H148" s="1" t="s">
-        <v>488</v>
+        <v>474</v>
       </c>
       <c r="I148" s="1" t="s">
         <v>72</v>
@@ -9732,33 +9894,33 @@
       <c r="M148" s="1"/>
       <c r="N148" s="1"/>
       <c r="O148" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="149" spans="1:15" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="149" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A149">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>489</v>
+        <v>475</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>485</v>
+        <v>471</v>
       </c>
       <c r="D149" s="1" t="s">
-        <v>486</v>
+        <v>472</v>
       </c>
       <c r="E149" t="s">
-        <v>490</v>
+        <v>476</v>
       </c>
       <c r="F149" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G149" t="s">
-        <v>870</v>
+        <v>866</v>
       </c>
       <c r="H149" s="1" t="s">
-        <v>491</v>
+        <v>477</v>
       </c>
       <c r="I149" s="1" t="s">
         <v>72</v>
@@ -9771,33 +9933,33 @@
       <c r="M149" s="1"/>
       <c r="N149" s="1"/>
       <c r="O149" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="150" spans="1:15" x14ac:dyDescent="0.25">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="150" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A150">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>492</v>
+        <v>478</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>485</v>
+        <v>471</v>
       </c>
       <c r="D150" s="1" t="s">
-        <v>486</v>
+        <v>472</v>
       </c>
       <c r="E150" t="s">
-        <v>493</v>
+        <v>479</v>
       </c>
       <c r="F150" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G150" t="s">
-        <v>871</v>
+        <v>867</v>
       </c>
       <c r="H150" s="1" t="s">
-        <v>494</v>
+        <v>480</v>
       </c>
       <c r="I150" s="1" t="s">
         <v>72</v>
@@ -9810,33 +9972,33 @@
       <c r="M150" s="1"/>
       <c r="N150" s="1"/>
       <c r="O150" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="151" spans="1:15" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="151" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A151">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>495</v>
+        <v>481</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>485</v>
+        <v>471</v>
       </c>
       <c r="D151" s="1" t="s">
-        <v>486</v>
+        <v>472</v>
       </c>
       <c r="E151" t="s">
-        <v>496</v>
+        <v>482</v>
       </c>
       <c r="F151" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G151" t="s">
-        <v>872</v>
+        <v>868</v>
       </c>
       <c r="H151" s="1" t="s">
-        <v>497</v>
+        <v>483</v>
       </c>
       <c r="I151" s="1" t="s">
         <v>72</v>
@@ -9849,15 +10011,15 @@
       <c r="M151" s="1"/>
       <c r="N151" s="1"/>
       <c r="O151" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="152" spans="1:15" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="152" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A152">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>498</v>
+        <v>484</v>
       </c>
       <c r="C152" s="1" t="s">
         <v>485</v>
@@ -9866,16 +10028,16 @@
         <v>486</v>
       </c>
       <c r="E152" t="s">
-        <v>499</v>
+        <v>487</v>
       </c>
       <c r="F152" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G152" t="s">
-        <v>873</v>
+        <v>869</v>
       </c>
       <c r="H152" s="1" t="s">
-        <v>500</v>
+        <v>488</v>
       </c>
       <c r="I152" s="1" t="s">
         <v>72</v>
@@ -9888,15 +10050,15 @@
       <c r="M152" s="1"/>
       <c r="N152" s="1"/>
       <c r="O152" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="153" spans="1:15" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="153" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A153">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>501</v>
+        <v>489</v>
       </c>
       <c r="C153" s="1" t="s">
         <v>485</v>
@@ -9905,16 +10067,16 @@
         <v>486</v>
       </c>
       <c r="E153" t="s">
-        <v>676</v>
+        <v>490</v>
       </c>
       <c r="F153" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G153" t="s">
-        <v>874</v>
+        <v>870</v>
       </c>
       <c r="H153" s="1" t="s">
-        <v>502</v>
+        <v>491</v>
       </c>
       <c r="I153" s="1" t="s">
         <v>72</v>
@@ -9927,15 +10089,15 @@
       <c r="M153" s="1"/>
       <c r="N153" s="1"/>
       <c r="O153" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="154" spans="1:15" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="154" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A154">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>503</v>
+        <v>492</v>
       </c>
       <c r="C154" s="1" t="s">
         <v>485</v>
@@ -9944,16 +10106,16 @@
         <v>486</v>
       </c>
       <c r="E154" t="s">
-        <v>677</v>
+        <v>493</v>
       </c>
       <c r="F154" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G154" t="s">
-        <v>875</v>
+        <v>871</v>
       </c>
       <c r="H154" s="1" t="s">
-        <v>504</v>
+        <v>494</v>
       </c>
       <c r="I154" s="1" t="s">
         <v>72</v>
@@ -9966,15 +10128,15 @@
       <c r="M154" s="1"/>
       <c r="N154" s="1"/>
       <c r="O154" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="155" spans="1:15" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="155" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A155">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>505</v>
+        <v>495</v>
       </c>
       <c r="C155" s="1" t="s">
         <v>485</v>
@@ -9983,16 +10145,16 @@
         <v>486</v>
       </c>
       <c r="E155" t="s">
-        <v>678</v>
+        <v>496</v>
       </c>
       <c r="F155" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G155" t="s">
-        <v>876</v>
+        <v>872</v>
       </c>
       <c r="H155" s="1" t="s">
-        <v>506</v>
+        <v>497</v>
       </c>
       <c r="I155" s="1" t="s">
         <v>72</v>
@@ -10005,15 +10167,15 @@
       <c r="M155" s="1"/>
       <c r="N155" s="1"/>
       <c r="O155" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="156" spans="1:15" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="156" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A156">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>507</v>
+        <v>498</v>
       </c>
       <c r="C156" s="1" t="s">
         <v>485</v>
@@ -10022,16 +10184,16 @@
         <v>486</v>
       </c>
       <c r="E156" t="s">
-        <v>508</v>
+        <v>499</v>
       </c>
       <c r="F156" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G156" t="s">
-        <v>877</v>
+        <v>873</v>
       </c>
       <c r="H156" s="1" t="s">
-        <v>509</v>
+        <v>500</v>
       </c>
       <c r="I156" s="1" t="s">
         <v>72</v>
@@ -10044,15 +10206,15 @@
       <c r="M156" s="1"/>
       <c r="N156" s="1"/>
       <c r="O156" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="157" spans="1:15" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="157" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A157">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>510</v>
+        <v>501</v>
       </c>
       <c r="C157" s="1" t="s">
         <v>485</v>
@@ -10061,16 +10223,16 @@
         <v>486</v>
       </c>
       <c r="E157" t="s">
-        <v>511</v>
+        <v>676</v>
       </c>
       <c r="F157" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G157" t="s">
-        <v>878</v>
+        <v>874</v>
       </c>
       <c r="H157" s="1" t="s">
-        <v>512</v>
+        <v>502</v>
       </c>
       <c r="I157" s="1" t="s">
         <v>72</v>
@@ -10083,15 +10245,15 @@
       <c r="M157" s="1"/>
       <c r="N157" s="1"/>
       <c r="O157" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="158" spans="1:15" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="158" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A158">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>539</v>
+        <v>503</v>
       </c>
       <c r="C158" s="1" t="s">
         <v>485</v>
@@ -10100,16 +10262,16 @@
         <v>486</v>
       </c>
       <c r="E158" t="s">
-        <v>544</v>
+        <v>677</v>
       </c>
       <c r="F158" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G158" t="s">
-        <v>879</v>
+        <v>875</v>
       </c>
       <c r="H158" s="1" t="s">
-        <v>880</v>
+        <v>504</v>
       </c>
       <c r="I158" s="1" t="s">
         <v>72</v>
@@ -10122,15 +10284,15 @@
       <c r="M158" s="1"/>
       <c r="N158" s="1"/>
       <c r="O158" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="159" spans="1:15" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="159" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A159">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>540</v>
+        <v>505</v>
       </c>
       <c r="C159" s="1" t="s">
         <v>485</v>
@@ -10139,16 +10301,16 @@
         <v>486</v>
       </c>
       <c r="E159" t="s">
-        <v>545</v>
+        <v>678</v>
       </c>
       <c r="F159" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G159" t="s">
-        <v>881</v>
+        <v>876</v>
       </c>
       <c r="H159" s="1" t="s">
-        <v>882</v>
+        <v>506</v>
       </c>
       <c r="I159" s="1" t="s">
         <v>72</v>
@@ -10161,15 +10323,15 @@
       <c r="M159" s="1"/>
       <c r="N159" s="1"/>
       <c r="O159" s="1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="160" spans="1:15" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="160" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A160">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>541</v>
+        <v>507</v>
       </c>
       <c r="C160" s="1" t="s">
         <v>485</v>
@@ -10178,16 +10340,16 @@
         <v>486</v>
       </c>
       <c r="E160" t="s">
-        <v>679</v>
+        <v>508</v>
       </c>
       <c r="F160" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G160" t="s">
-        <v>883</v>
+        <v>877</v>
       </c>
       <c r="H160" s="1" t="s">
-        <v>884</v>
+        <v>509</v>
       </c>
       <c r="I160" s="1" t="s">
         <v>72</v>
@@ -10200,15 +10362,15 @@
       <c r="M160" s="1"/>
       <c r="N160" s="1"/>
       <c r="O160" s="1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="161" spans="1:15" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="161" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A161">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>542</v>
+        <v>510</v>
       </c>
       <c r="C161" s="1" t="s">
         <v>485</v>
@@ -10217,16 +10379,16 @@
         <v>486</v>
       </c>
       <c r="E161" t="s">
-        <v>680</v>
+        <v>511</v>
       </c>
       <c r="F161" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G161" t="s">
-        <v>885</v>
+        <v>878</v>
       </c>
       <c r="H161" s="1" t="s">
-        <v>886</v>
+        <v>512</v>
       </c>
       <c r="I161" s="1" t="s">
         <v>72</v>
@@ -10239,15 +10401,15 @@
       <c r="M161" s="1"/>
       <c r="N161" s="1"/>
       <c r="O161" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="162" spans="1:15" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="162" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A162">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>543</v>
+        <v>539</v>
       </c>
       <c r="C162" s="1" t="s">
         <v>485</v>
@@ -10256,16 +10418,16 @@
         <v>486</v>
       </c>
       <c r="E162" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="F162" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G162" t="s">
-        <v>887</v>
+        <v>879</v>
       </c>
       <c r="H162" s="1" t="s">
-        <v>888</v>
+        <v>880</v>
       </c>
       <c r="I162" s="1" t="s">
         <v>72</v>
@@ -10278,15 +10440,15 @@
       <c r="M162" s="1"/>
       <c r="N162" s="1"/>
       <c r="O162" s="1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="163" spans="1:15" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="163" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A163">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>889</v>
+        <v>540</v>
       </c>
       <c r="C163" s="1" t="s">
         <v>485</v>
@@ -10294,24 +10456,38 @@
       <c r="D163" s="1" t="s">
         <v>486</v>
       </c>
+      <c r="E163" t="s">
+        <v>545</v>
+      </c>
       <c r="F163" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H163" s="1"/>
-      <c r="I163" s="1"/>
+      <c r="G163" t="s">
+        <v>881</v>
+      </c>
+      <c r="H163" s="1" t="s">
+        <v>882</v>
+      </c>
+      <c r="I163" s="1" t="s">
+        <v>72</v>
+      </c>
       <c r="J163" s="1"/>
       <c r="K163" s="1"/>
-      <c r="L163" s="1"/>
+      <c r="L163" s="1" t="s">
+        <v>73</v>
+      </c>
       <c r="M163" s="1"/>
       <c r="N163" s="1"/>
-      <c r="O163" s="1"/>
-    </row>
-    <row r="164" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O163" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="164" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A164">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>890</v>
+        <v>541</v>
       </c>
       <c r="C164" s="1" t="s">
         <v>485</v>
@@ -10319,40 +10495,56 @@
       <c r="D164" s="1" t="s">
         <v>486</v>
       </c>
+      <c r="E164" t="s">
+        <v>679</v>
+      </c>
       <c r="F164" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H164" s="1"/>
-      <c r="I164" s="1"/>
+      <c r="G164" t="s">
+        <v>883</v>
+      </c>
+      <c r="H164" s="1" t="s">
+        <v>884</v>
+      </c>
+      <c r="I164" s="1" t="s">
+        <v>72</v>
+      </c>
       <c r="J164" s="1"/>
       <c r="K164" s="1"/>
-      <c r="L164" s="1"/>
+      <c r="L164" s="1" t="s">
+        <v>73</v>
+      </c>
       <c r="M164" s="1"/>
       <c r="N164" s="1"/>
-      <c r="O164" s="1"/>
-    </row>
-    <row r="165" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O164" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="165" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A165">
-        <v>301</v>
+        <v>218</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>513</v>
+        <v>542</v>
       </c>
       <c r="C165" s="1" t="s">
-        <v>514</v>
+        <v>485</v>
       </c>
       <c r="D165" s="1" t="s">
-        <v>514</v>
-      </c>
-      <c r="E165" s="1" t="s">
-        <v>514</v>
+        <v>486</v>
+      </c>
+      <c r="E165" t="s">
+        <v>680</v>
       </c>
       <c r="F165" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G165" s="1"/>
+      <c r="G165" t="s">
+        <v>885</v>
+      </c>
       <c r="H165" s="1" t="s">
-        <v>515</v>
+        <v>886</v>
       </c>
       <c r="I165" s="1" t="s">
         <v>72</v>
@@ -10365,6 +10557,152 @@
       <c r="M165" s="1"/>
       <c r="N165" s="1"/>
       <c r="O165" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="166" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A166">
+        <v>219</v>
+      </c>
+      <c r="B166" s="1" t="s">
+        <v>543</v>
+      </c>
+      <c r="C166" s="1" t="s">
+        <v>485</v>
+      </c>
+      <c r="D166" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="E166" t="s">
+        <v>546</v>
+      </c>
+      <c r="F166" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G166" t="s">
+        <v>887</v>
+      </c>
+      <c r="H166" s="1" t="s">
+        <v>888</v>
+      </c>
+      <c r="I166" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J166" s="1"/>
+      <c r="K166" s="1"/>
+      <c r="L166" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="M166" s="1"/>
+      <c r="N166" s="1"/>
+      <c r="O166" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="167" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A167">
+        <v>220</v>
+      </c>
+      <c r="B167" s="1" t="s">
+        <v>889</v>
+      </c>
+      <c r="C167" s="1" t="s">
+        <v>485</v>
+      </c>
+      <c r="D167" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="F167" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H167" s="1"/>
+      <c r="I167" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J167" s="1"/>
+      <c r="K167" s="1"/>
+      <c r="L167" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="M167" s="1"/>
+      <c r="N167" s="1"/>
+      <c r="O167" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="168" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A168">
+        <v>221</v>
+      </c>
+      <c r="B168" s="1" t="s">
+        <v>890</v>
+      </c>
+      <c r="C168" s="1" t="s">
+        <v>485</v>
+      </c>
+      <c r="D168" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="E168" t="s">
+        <v>959</v>
+      </c>
+      <c r="F168" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G168" t="s">
+        <v>958</v>
+      </c>
+      <c r="H168" s="1" t="s">
+        <v>960</v>
+      </c>
+      <c r="I168" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J168" s="1"/>
+      <c r="K168" s="1"/>
+      <c r="L168" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="M168" s="1"/>
+      <c r="N168" s="1"/>
+      <c r="O168" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="169" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A169">
+        <v>301</v>
+      </c>
+      <c r="B169" s="1" t="s">
+        <v>513</v>
+      </c>
+      <c r="C169" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="D169" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="E169" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="F169" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G169" s="1"/>
+      <c r="H169" s="1" t="s">
+        <v>515</v>
+      </c>
+      <c r="I169" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J169" s="1"/>
+      <c r="K169" s="1"/>
+      <c r="L169" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="M169" s="1"/>
+      <c r="N169" s="1"/>
+      <c r="O169" s="1" t="s">
         <v>144</v>
       </c>
     </row>

</xml_diff>

<commit_message>
refactor java.util.Date  to java time fix *nix/mac launcher script issue
</commit_message>
<xml_diff>
--- a/src/main/resources/AlertMessageList.xlsx
+++ b/src/main/resources/AlertMessageList.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_PRIVATE\Github_Master\pega-logviewer\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2580C9B5-18A9-475F-9D4E-450195B1287B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8872A174-D598-4070-850C-9479E4592321}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{10474AC9-EC98-4A01-86DB-DE0ABEBDFAED}"/>
+    <workbookView xWindow="-28920" yWindow="15" windowWidth="29040" windowHeight="17520" xr2:uid="{10474AC9-EC98-4A01-86DB-DE0ABEBDFAED}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2027" uniqueCount="961">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2148" uniqueCount="987">
   <si>
     <t>Id</t>
   </si>
@@ -2911,6 +2911,84 @@
   </si>
   <si>
     <t>The system generates security alert SECU0021 when an attempt has been made to import an expired certificate into the platform truststore.</t>
+  </si>
+  <si>
+    <t>PEGA0148</t>
+  </si>
+  <si>
+    <t>PEGA0149</t>
+  </si>
+  <si>
+    <t>PEGA0150</t>
+  </si>
+  <si>
+    <t>PEGA0151</t>
+  </si>
+  <si>
+    <t>PEGA0152</t>
+  </si>
+  <si>
+    <t>PEGA0153</t>
+  </si>
+  <si>
+    <t>PEGA0154</t>
+  </si>
+  <si>
+    <t>PEGA0155</t>
+  </si>
+  <si>
+    <t>PEGA0156</t>
+  </si>
+  <si>
+    <t>PEGA0157</t>
+  </si>
+  <si>
+    <t>PEGA0158</t>
+  </si>
+  <si>
+    <t>PEGA0159</t>
+  </si>
+  <si>
+    <t>PEGA0160</t>
+  </si>
+  <si>
+    <t>PEGA0161</t>
+  </si>
+  <si>
+    <t>PEGA0162</t>
+  </si>
+  <si>
+    <t>PEGA0163</t>
+  </si>
+  <si>
+    <t>ADM model update time</t>
+  </si>
+  <si>
+    <t>DSM Adaptive Decision Manager</t>
+  </si>
+  <si>
+    <t>https://docs.pega.com/bundle/alerts/page/platform/alerts/pega0146-alert-adm-model-update.html</t>
+  </si>
+  <si>
+    <t>The Adaptive Decision Manager (ADM) triggers the PEGA0146 alert when an adaptive model update exceeds the update interval configured for the system.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Adaptive Decision Manager (ADM) triggers the PEGA0147 alert when an adaptive model has not received any responses for a period that exceeds the threshold, which by default is 24 hours. </t>
+  </si>
+  <si>
+    <t>https://docs.pega.com/bundle/alerts/page/platform/alerts/pega0147-alert-model-not-updated.html</t>
+  </si>
+  <si>
+    <t>ADM model not updated</t>
+  </si>
+  <si>
+    <t>Long running ADM model persist operation</t>
+  </si>
+  <si>
+    <t>https://docs.pega.com/bundle/alerts/page/platform/alerts/pega0160-long-running-adm-model-persist-operation.html</t>
+  </si>
+  <si>
+    <t>The Adaptive Decision Manager (ADM) triggers the PEGA0160 alert when an adaptive model persist operation is taking longer than the threshold, which by default is 30 seconds. This alert indicates that operations are slower than expected and can cause adaptive model updates to complete less frequent than they should.</t>
   </si>
 </sst>
 </file>
@@ -2958,10 +3036,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3068,8 +3147,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{179863B1-6A76-4246-A1BC-FE8FC898012F}" name="Table1" displayName="Table1" ref="A1:O169" tableType="xml" totalsRowShown="0" connectionId="1">
-  <autoFilter ref="A1:O169" xr:uid="{4F6276EB-680B-458A-B167-A8C1331B3E93}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{179863B1-6A76-4246-A1BC-FE8FC898012F}" name="Table1" displayName="Table1" ref="A1:O185" tableType="xml" totalsRowShown="0" connectionId="1">
+  <autoFilter ref="A1:O185" xr:uid="{4F6276EB-680B-458A-B167-A8C1331B3E93}"/>
   <tableColumns count="15">
     <tableColumn id="1" xr3:uid="{39609868-3AA4-445A-A488-970B25180B73}" uniqueName="Id" name="Id">
       <xmlColumnPr mapId="1" xpath="/AlertMessageList/AlertMessage/Id" xmlDataType="int"/>
@@ -3418,34 +3497,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O169"/>
+  <dimension ref="A1:O185"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A127" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A125" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
       <selection activeCell="A82" sqref="A82"/>
-      <selection pane="topRight" activeCell="A173" sqref="A173"/>
+      <selection pane="topRight" activeCell="H161" sqref="H161"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13" customWidth="1"/>
-    <col min="4" max="4" width="35.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="60.453125" customWidth="1"/>
-    <col min="6" max="6" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="100.1796875" customWidth="1"/>
-    <col min="8" max="8" width="141.7265625" customWidth="1"/>
-    <col min="9" max="9" width="48.81640625" customWidth="1"/>
-    <col min="10" max="10" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="61.26953125" customWidth="1"/>
-    <col min="12" max="12" width="15.81640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="24.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="60.42578125" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="100.140625" customWidth="1"/>
+    <col min="8" max="8" width="141.7109375" customWidth="1"/>
+    <col min="9" max="9" width="48.85546875" customWidth="1"/>
+    <col min="10" max="10" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="61.28515625" customWidth="1"/>
+    <col min="12" max="12" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="24.5703125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="49" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3492,7 +3571,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3539,7 +3618,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3586,7 +3665,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3633,7 +3712,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -3680,7 +3759,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -3727,7 +3806,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -3766,7 +3845,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -3805,7 +3884,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -3844,7 +3923,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -3883,7 +3962,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -3922,7 +4001,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -3969,7 +4048,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -4008,7 +4087,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -4047,7 +4126,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -4086,7 +4165,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -4125,7 +4204,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -4170,7 +4249,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -4215,7 +4294,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -4262,7 +4341,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -4309,7 +4388,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -4356,7 +4435,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -4403,7 +4482,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -4448,7 +4527,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -4493,7 +4572,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -4540,7 +4619,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -4587,7 +4666,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -4632,7 +4711,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -4677,7 +4756,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -4712,7 +4791,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -4759,7 +4838,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -4806,7 +4885,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -4841,7 +4920,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -4888,7 +4967,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -4935,7 +5014,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -4982,7 +5061,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -5029,7 +5108,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -5070,7 +5149,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -5117,7 +5196,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -5164,7 +5243,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -5211,7 +5290,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -5258,7 +5337,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -5305,7 +5384,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -5352,7 +5431,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -5399,7 +5478,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -5446,7 +5525,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
@@ -5493,7 +5572,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
@@ -5540,7 +5619,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -5587,7 +5666,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
@@ -5634,7 +5713,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
@@ -5681,7 +5760,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
@@ -5728,7 +5807,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
@@ -5771,7 +5850,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
@@ -5818,7 +5897,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
@@ -5865,7 +5944,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
@@ -5912,7 +5991,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
@@ -5959,7 +6038,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
@@ -6006,7 +6085,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>58</v>
       </c>
@@ -6053,7 +6132,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>59</v>
       </c>
@@ -6100,7 +6179,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>60</v>
       </c>
@@ -6147,7 +6226,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>61</v>
       </c>
@@ -6194,7 +6273,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>62</v>
       </c>
@@ -6241,7 +6320,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>63</v>
       </c>
@@ -6288,7 +6367,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>64</v>
       </c>
@@ -6335,7 +6414,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>65</v>
       </c>
@@ -6382,7 +6461,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>66</v>
       </c>
@@ -6425,7 +6504,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>67</v>
       </c>
@@ -6472,7 +6551,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>68</v>
       </c>
@@ -6519,7 +6598,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>69</v>
       </c>
@@ -6566,7 +6645,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>70</v>
       </c>
@@ -6613,7 +6692,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>71</v>
       </c>
@@ -6660,7 +6739,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>72</v>
       </c>
@@ -6707,7 +6786,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>73</v>
       </c>
@@ -6754,7 +6833,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>74</v>
       </c>
@@ -6801,7 +6880,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>75</v>
       </c>
@@ -6848,7 +6927,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>76</v>
       </c>
@@ -6895,7 +6974,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>77</v>
       </c>
@@ -6942,7 +7021,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>78</v>
       </c>
@@ -6989,7 +7068,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>79</v>
       </c>
@@ -7036,7 +7115,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>80</v>
       </c>
@@ -7083,7 +7162,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="81" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>81</v>
       </c>
@@ -7130,7 +7209,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="82" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>82</v>
       </c>
@@ -7177,7 +7256,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="83" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>83</v>
       </c>
@@ -7224,7 +7303,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="84" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>84</v>
       </c>
@@ -7269,7 +7348,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="85" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>85</v>
       </c>
@@ -7316,7 +7395,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="86" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>86</v>
       </c>
@@ -7363,7 +7442,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="87" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>87</v>
       </c>
@@ -7410,7 +7489,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="88" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>88</v>
       </c>
@@ -7449,7 +7528,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="89" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>89</v>
       </c>
@@ -7488,7 +7567,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="90" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>90</v>
       </c>
@@ -7527,7 +7606,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="91" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>91</v>
       </c>
@@ -7566,7 +7645,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="92" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>92</v>
       </c>
@@ -7613,7 +7692,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="93" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>93</v>
       </c>
@@ -7660,7 +7739,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="94" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>94</v>
       </c>
@@ -7703,7 +7782,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="95" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>95</v>
       </c>
@@ -7748,7 +7827,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="96" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>96</v>
       </c>
@@ -7793,7 +7872,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="97" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>97</v>
       </c>
@@ -7840,7 +7919,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="98" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>98</v>
       </c>
@@ -7879,7 +7958,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="99" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>99</v>
       </c>
@@ -7918,7 +7997,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="100" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>100</v>
       </c>
@@ -7957,7 +8036,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="101" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>101</v>
       </c>
@@ -7996,7 +8075,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="102" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>102</v>
       </c>
@@ -8035,7 +8114,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="103" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>103</v>
       </c>
@@ -8074,7 +8153,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="104" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>104</v>
       </c>
@@ -8113,7 +8192,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="105" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>105</v>
       </c>
@@ -8160,7 +8239,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="106" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>106</v>
       </c>
@@ -8199,7 +8278,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="107" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>107</v>
       </c>
@@ -8246,7 +8325,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="108" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>108</v>
       </c>
@@ -8283,7 +8362,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="109" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>109</v>
       </c>
@@ -8330,7 +8409,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="110" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>110</v>
       </c>
@@ -8377,7 +8456,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="111" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>111</v>
       </c>
@@ -8418,7 +8497,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="112" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>112</v>
       </c>
@@ -8459,7 +8538,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="113" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>113</v>
       </c>
@@ -8500,7 +8579,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="114" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>114</v>
       </c>
@@ -8541,7 +8620,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="115" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>115</v>
       </c>
@@ -8582,7 +8661,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="116" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>116</v>
       </c>
@@ -8623,7 +8702,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="117" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>117</v>
       </c>
@@ -8664,7 +8743,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="118" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>118</v>
       </c>
@@ -8705,7 +8784,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="119" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>119</v>
       </c>
@@ -8752,7 +8831,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="120" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>120</v>
       </c>
@@ -8795,7 +8874,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="121" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>121</v>
       </c>
@@ -8836,7 +8915,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="122" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>122</v>
       </c>
@@ -8873,7 +8952,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="123" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>123</v>
       </c>
@@ -8910,7 +8989,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="124" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>124</v>
       </c>
@@ -8947,7 +9026,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="125" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>125</v>
       </c>
@@ -8986,7 +9065,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="126" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>126</v>
       </c>
@@ -9025,7 +9104,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="127" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>127</v>
       </c>
@@ -9064,7 +9143,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="128" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>128</v>
       </c>
@@ -9103,7 +9182,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="129" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>129</v>
       </c>
@@ -9150,7 +9229,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="130" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>130</v>
       </c>
@@ -9197,7 +9276,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="131" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>131</v>
       </c>
@@ -9236,7 +9315,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="132" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>132</v>
       </c>
@@ -9275,7 +9354,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="133" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>133</v>
       </c>
@@ -9314,7 +9393,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="134" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>134</v>
       </c>
@@ -9355,7 +9434,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="135" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>135</v>
       </c>
@@ -9396,7 +9475,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="136" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>136</v>
       </c>
@@ -9437,7 +9516,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="137" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>137</v>
       </c>
@@ -9480,7 +9559,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="138" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>138</v>
       </c>
@@ -9521,7 +9600,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="139" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>139</v>
       </c>
@@ -9562,7 +9641,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="140" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>140</v>
       </c>
@@ -9603,7 +9682,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="141" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>141</v>
       </c>
@@ -9644,7 +9723,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="142" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>142</v>
       </c>
@@ -9685,7 +9764,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="143" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>143</v>
       </c>
@@ -9726,7 +9805,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="144" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>144</v>
       </c>
@@ -9759,7 +9838,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="145" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>145</v>
       </c>
@@ -9792,7 +9871,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="146" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>146</v>
       </c>
@@ -9803,14 +9882,20 @@
         <v>17</v>
       </c>
       <c r="D146" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="E146" s="1"/>
+        <v>978</v>
+      </c>
+      <c r="E146" s="1" t="s">
+        <v>977</v>
+      </c>
       <c r="F146" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G146" s="1"/>
-      <c r="H146" s="1"/>
+      <c r="G146" s="3" t="s">
+        <v>979</v>
+      </c>
+      <c r="H146" s="1" t="s">
+        <v>980</v>
+      </c>
       <c r="I146" s="1" t="s">
         <v>72</v>
       </c>
@@ -9825,7 +9910,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="147" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>147</v>
       </c>
@@ -9836,14 +9921,20 @@
         <v>17</v>
       </c>
       <c r="D147" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="E147" s="1"/>
+        <v>978</v>
+      </c>
+      <c r="E147" s="1" t="s">
+        <v>983</v>
+      </c>
       <c r="F147" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G147" s="1"/>
-      <c r="H147" s="1"/>
+      <c r="G147" s="1" t="s">
+        <v>982</v>
+      </c>
+      <c r="H147" s="1" t="s">
+        <v>981</v>
+      </c>
       <c r="I147" s="1" t="s">
         <v>72</v>
       </c>
@@ -9858,31 +9949,25 @@
         <v>144</v>
       </c>
     </row>
-    <row r="148" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A148">
-        <v>201</v>
+        <v>148</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>470</v>
+        <v>961</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>471</v>
+        <v>17</v>
       </c>
       <c r="D148" s="1" t="s">
-        <v>472</v>
-      </c>
-      <c r="E148" t="s">
-        <v>473</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="E148" s="1"/>
       <c r="F148" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G148" t="s">
-        <v>865</v>
-      </c>
-      <c r="H148" s="1" t="s">
-        <v>474</v>
-      </c>
+      <c r="G148" s="1"/>
+      <c r="H148" s="1"/>
       <c r="I148" s="1" t="s">
         <v>72</v>
       </c>
@@ -9894,34 +9979,28 @@
       <c r="M148" s="1"/>
       <c r="N148" s="1"/>
       <c r="O148" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="149" spans="1:15" x14ac:dyDescent="0.35">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="149" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A149">
-        <v>202</v>
+        <v>149</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>475</v>
+        <v>962</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>471</v>
+        <v>17</v>
       </c>
       <c r="D149" s="1" t="s">
-        <v>472</v>
-      </c>
-      <c r="E149" t="s">
-        <v>476</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="E149" s="1"/>
       <c r="F149" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G149" t="s">
-        <v>866</v>
-      </c>
-      <c r="H149" s="1" t="s">
-        <v>477</v>
-      </c>
+      <c r="G149" s="1"/>
+      <c r="H149" s="1"/>
       <c r="I149" s="1" t="s">
         <v>72</v>
       </c>
@@ -9933,34 +10012,28 @@
       <c r="M149" s="1"/>
       <c r="N149" s="1"/>
       <c r="O149" s="1" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="150" spans="1:15" x14ac:dyDescent="0.35">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="150" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A150">
-        <v>203</v>
+        <v>150</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>478</v>
+        <v>963</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>471</v>
+        <v>17</v>
       </c>
       <c r="D150" s="1" t="s">
-        <v>472</v>
-      </c>
-      <c r="E150" t="s">
-        <v>479</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="E150" s="1"/>
       <c r="F150" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G150" t="s">
-        <v>867</v>
-      </c>
-      <c r="H150" s="1" t="s">
-        <v>480</v>
-      </c>
+      <c r="G150" s="1"/>
+      <c r="H150" s="1"/>
       <c r="I150" s="1" t="s">
         <v>72</v>
       </c>
@@ -9972,34 +10045,28 @@
       <c r="M150" s="1"/>
       <c r="N150" s="1"/>
       <c r="O150" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="151" spans="1:15" x14ac:dyDescent="0.35">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="151" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A151">
-        <v>204</v>
+        <v>151</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>481</v>
+        <v>964</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>471</v>
+        <v>17</v>
       </c>
       <c r="D151" s="1" t="s">
-        <v>472</v>
-      </c>
-      <c r="E151" t="s">
-        <v>482</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="E151" s="1"/>
       <c r="F151" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G151" t="s">
-        <v>868</v>
-      </c>
-      <c r="H151" s="1" t="s">
-        <v>483</v>
-      </c>
+      <c r="G151" s="1"/>
+      <c r="H151" s="1"/>
       <c r="I151" s="1" t="s">
         <v>72</v>
       </c>
@@ -10011,34 +10078,28 @@
       <c r="M151" s="1"/>
       <c r="N151" s="1"/>
       <c r="O151" s="1" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="152" spans="1:15" x14ac:dyDescent="0.35">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="152" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A152">
-        <v>205</v>
+        <v>152</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>484</v>
+        <v>965</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>485</v>
+        <v>17</v>
       </c>
       <c r="D152" s="1" t="s">
-        <v>486</v>
-      </c>
-      <c r="E152" t="s">
-        <v>487</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="E152" s="1"/>
       <c r="F152" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G152" t="s">
-        <v>869</v>
-      </c>
-      <c r="H152" s="1" t="s">
-        <v>488</v>
-      </c>
+      <c r="G152" s="1"/>
+      <c r="H152" s="1"/>
       <c r="I152" s="1" t="s">
         <v>72</v>
       </c>
@@ -10050,34 +10111,28 @@
       <c r="M152" s="1"/>
       <c r="N152" s="1"/>
       <c r="O152" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="153" spans="1:15" x14ac:dyDescent="0.35">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="153" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A153">
-        <v>206</v>
+        <v>153</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>489</v>
+        <v>966</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>485</v>
+        <v>17</v>
       </c>
       <c r="D153" s="1" t="s">
-        <v>486</v>
-      </c>
-      <c r="E153" t="s">
-        <v>490</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="E153" s="1"/>
       <c r="F153" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G153" t="s">
-        <v>870</v>
-      </c>
-      <c r="H153" s="1" t="s">
-        <v>491</v>
-      </c>
+      <c r="G153" s="1"/>
+      <c r="H153" s="1"/>
       <c r="I153" s="1" t="s">
         <v>72</v>
       </c>
@@ -10089,34 +10144,28 @@
       <c r="M153" s="1"/>
       <c r="N153" s="1"/>
       <c r="O153" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="154" spans="1:15" x14ac:dyDescent="0.35">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="154" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A154">
-        <v>207</v>
+        <v>154</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>492</v>
+        <v>967</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>485</v>
+        <v>17</v>
       </c>
       <c r="D154" s="1" t="s">
-        <v>486</v>
-      </c>
-      <c r="E154" t="s">
-        <v>493</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="E154" s="1"/>
       <c r="F154" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G154" t="s">
-        <v>871</v>
-      </c>
-      <c r="H154" s="1" t="s">
-        <v>494</v>
-      </c>
+      <c r="G154" s="1"/>
+      <c r="H154" s="1"/>
       <c r="I154" s="1" t="s">
         <v>72</v>
       </c>
@@ -10128,34 +10177,28 @@
       <c r="M154" s="1"/>
       <c r="N154" s="1"/>
       <c r="O154" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="155" spans="1:15" x14ac:dyDescent="0.35">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="155" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A155">
-        <v>208</v>
+        <v>155</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>495</v>
+        <v>968</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>485</v>
+        <v>17</v>
       </c>
       <c r="D155" s="1" t="s">
-        <v>486</v>
-      </c>
-      <c r="E155" t="s">
-        <v>496</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="E155" s="1"/>
       <c r="F155" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G155" t="s">
-        <v>872</v>
-      </c>
-      <c r="H155" s="1" t="s">
-        <v>497</v>
-      </c>
+      <c r="G155" s="1"/>
+      <c r="H155" s="1"/>
       <c r="I155" s="1" t="s">
         <v>72</v>
       </c>
@@ -10167,34 +10210,28 @@
       <c r="M155" s="1"/>
       <c r="N155" s="1"/>
       <c r="O155" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="156" spans="1:15" x14ac:dyDescent="0.35">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="156" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A156">
-        <v>209</v>
+        <v>156</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>498</v>
+        <v>969</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>485</v>
+        <v>17</v>
       </c>
       <c r="D156" s="1" t="s">
-        <v>486</v>
-      </c>
-      <c r="E156" t="s">
-        <v>499</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="E156" s="1"/>
       <c r="F156" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G156" t="s">
-        <v>873</v>
-      </c>
-      <c r="H156" s="1" t="s">
-        <v>500</v>
-      </c>
+      <c r="G156" s="1"/>
+      <c r="H156" s="1"/>
       <c r="I156" s="1" t="s">
         <v>72</v>
       </c>
@@ -10206,34 +10243,28 @@
       <c r="M156" s="1"/>
       <c r="N156" s="1"/>
       <c r="O156" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="157" spans="1:15" x14ac:dyDescent="0.35">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="157" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A157">
-        <v>210</v>
+        <v>157</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>501</v>
+        <v>970</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>485</v>
+        <v>17</v>
       </c>
       <c r="D157" s="1" t="s">
-        <v>486</v>
-      </c>
-      <c r="E157" t="s">
-        <v>676</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="E157" s="1"/>
       <c r="F157" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G157" t="s">
-        <v>874</v>
-      </c>
-      <c r="H157" s="1" t="s">
-        <v>502</v>
-      </c>
+      <c r="G157" s="1"/>
+      <c r="H157" s="1"/>
       <c r="I157" s="1" t="s">
         <v>72</v>
       </c>
@@ -10245,34 +10276,28 @@
       <c r="M157" s="1"/>
       <c r="N157" s="1"/>
       <c r="O157" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="158" spans="1:15" x14ac:dyDescent="0.35">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="158" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A158">
-        <v>211</v>
+        <v>158</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>503</v>
+        <v>971</v>
       </c>
       <c r="C158" s="1" t="s">
-        <v>485</v>
+        <v>17</v>
       </c>
       <c r="D158" s="1" t="s">
-        <v>486</v>
-      </c>
-      <c r="E158" t="s">
-        <v>677</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="E158" s="1"/>
       <c r="F158" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G158" t="s">
-        <v>875</v>
-      </c>
-      <c r="H158" s="1" t="s">
-        <v>504</v>
-      </c>
+      <c r="G158" s="1"/>
+      <c r="H158" s="1"/>
       <c r="I158" s="1" t="s">
         <v>72</v>
       </c>
@@ -10284,34 +10309,28 @@
       <c r="M158" s="1"/>
       <c r="N158" s="1"/>
       <c r="O158" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="159" spans="1:15" x14ac:dyDescent="0.35">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="159" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A159">
-        <v>212</v>
+        <v>159</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>505</v>
+        <v>972</v>
       </c>
       <c r="C159" s="1" t="s">
-        <v>485</v>
+        <v>17</v>
       </c>
       <c r="D159" s="1" t="s">
-        <v>486</v>
-      </c>
-      <c r="E159" t="s">
-        <v>678</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="E159" s="1"/>
       <c r="F159" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G159" t="s">
-        <v>876</v>
-      </c>
-      <c r="H159" s="1" t="s">
-        <v>506</v>
-      </c>
+      <c r="G159" s="1"/>
+      <c r="H159" s="1"/>
       <c r="I159" s="1" t="s">
         <v>72</v>
       </c>
@@ -10323,33 +10342,33 @@
       <c r="M159" s="1"/>
       <c r="N159" s="1"/>
       <c r="O159" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="160" spans="1:15" x14ac:dyDescent="0.35">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="160" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A160">
-        <v>213</v>
+        <v>160</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>507</v>
+        <v>973</v>
       </c>
       <c r="C160" s="1" t="s">
-        <v>485</v>
+        <v>17</v>
       </c>
       <c r="D160" s="1" t="s">
-        <v>486</v>
-      </c>
-      <c r="E160" t="s">
-        <v>508</v>
+        <v>978</v>
+      </c>
+      <c r="E160" s="1" t="s">
+        <v>984</v>
       </c>
       <c r="F160" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G160" t="s">
-        <v>877</v>
+      <c r="G160" s="1" t="s">
+        <v>985</v>
       </c>
       <c r="H160" s="1" t="s">
-        <v>509</v>
+        <v>986</v>
       </c>
       <c r="I160" s="1" t="s">
         <v>72</v>
@@ -10362,34 +10381,28 @@
       <c r="M160" s="1"/>
       <c r="N160" s="1"/>
       <c r="O160" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="161" spans="1:15" x14ac:dyDescent="0.35">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="161" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A161">
-        <v>214</v>
+        <v>161</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>510</v>
+        <v>974</v>
       </c>
       <c r="C161" s="1" t="s">
-        <v>485</v>
+        <v>17</v>
       </c>
       <c r="D161" s="1" t="s">
-        <v>486</v>
-      </c>
-      <c r="E161" t="s">
-        <v>511</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="E161" s="1"/>
       <c r="F161" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G161" t="s">
-        <v>878</v>
-      </c>
-      <c r="H161" s="1" t="s">
-        <v>512</v>
-      </c>
+      <c r="G161" s="1"/>
+      <c r="H161" s="1"/>
       <c r="I161" s="1" t="s">
         <v>72</v>
       </c>
@@ -10401,34 +10414,28 @@
       <c r="M161" s="1"/>
       <c r="N161" s="1"/>
       <c r="O161" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="162" spans="1:15" x14ac:dyDescent="0.35">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="162" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A162">
-        <v>215</v>
+        <v>162</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>539</v>
+        <v>975</v>
       </c>
       <c r="C162" s="1" t="s">
-        <v>485</v>
+        <v>17</v>
       </c>
       <c r="D162" s="1" t="s">
-        <v>486</v>
-      </c>
-      <c r="E162" t="s">
-        <v>544</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="E162" s="1"/>
       <c r="F162" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G162" t="s">
-        <v>879</v>
-      </c>
-      <c r="H162" s="1" t="s">
-        <v>880</v>
-      </c>
+      <c r="G162" s="1"/>
+      <c r="H162" s="1"/>
       <c r="I162" s="1" t="s">
         <v>72</v>
       </c>
@@ -10440,34 +10447,28 @@
       <c r="M162" s="1"/>
       <c r="N162" s="1"/>
       <c r="O162" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="163" spans="1:15" x14ac:dyDescent="0.35">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="163" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A163">
-        <v>216</v>
+        <v>163</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>540</v>
+        <v>976</v>
       </c>
       <c r="C163" s="1" t="s">
-        <v>485</v>
+        <v>17</v>
       </c>
       <c r="D163" s="1" t="s">
-        <v>486</v>
-      </c>
-      <c r="E163" t="s">
-        <v>545</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="E163" s="1"/>
       <c r="F163" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G163" t="s">
-        <v>881</v>
-      </c>
-      <c r="H163" s="1" t="s">
-        <v>882</v>
-      </c>
+      <c r="G163" s="1"/>
+      <c r="H163" s="1"/>
       <c r="I163" s="1" t="s">
         <v>72</v>
       </c>
@@ -10479,33 +10480,33 @@
       <c r="M163" s="1"/>
       <c r="N163" s="1"/>
       <c r="O163" s="1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="164" spans="1:15" x14ac:dyDescent="0.35">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="164" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A164">
-        <v>217</v>
+        <v>201</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>541</v>
+        <v>470</v>
       </c>
       <c r="C164" s="1" t="s">
-        <v>485</v>
+        <v>471</v>
       </c>
       <c r="D164" s="1" t="s">
-        <v>486</v>
+        <v>472</v>
       </c>
       <c r="E164" t="s">
-        <v>679</v>
+        <v>473</v>
       </c>
       <c r="F164" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G164" t="s">
-        <v>883</v>
+        <v>865</v>
       </c>
       <c r="H164" s="1" t="s">
-        <v>884</v>
+        <v>474</v>
       </c>
       <c r="I164" s="1" t="s">
         <v>72</v>
@@ -10518,33 +10519,33 @@
       <c r="M164" s="1"/>
       <c r="N164" s="1"/>
       <c r="O164" s="1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="165" spans="1:15" x14ac:dyDescent="0.35">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="165" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A165">
-        <v>218</v>
+        <v>202</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>542</v>
+        <v>475</v>
       </c>
       <c r="C165" s="1" t="s">
-        <v>485</v>
+        <v>471</v>
       </c>
       <c r="D165" s="1" t="s">
-        <v>486</v>
+        <v>472</v>
       </c>
       <c r="E165" t="s">
-        <v>680</v>
+        <v>476</v>
       </c>
       <c r="F165" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G165" t="s">
-        <v>885</v>
+        <v>866</v>
       </c>
       <c r="H165" s="1" t="s">
-        <v>886</v>
+        <v>477</v>
       </c>
       <c r="I165" s="1" t="s">
         <v>72</v>
@@ -10557,33 +10558,33 @@
       <c r="M165" s="1"/>
       <c r="N165" s="1"/>
       <c r="O165" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="166" spans="1:15" x14ac:dyDescent="0.35">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="166" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A166">
-        <v>219</v>
+        <v>203</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>543</v>
+        <v>478</v>
       </c>
       <c r="C166" s="1" t="s">
-        <v>485</v>
+        <v>471</v>
       </c>
       <c r="D166" s="1" t="s">
-        <v>486</v>
+        <v>472</v>
       </c>
       <c r="E166" t="s">
-        <v>546</v>
+        <v>479</v>
       </c>
       <c r="F166" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G166" t="s">
-        <v>887</v>
+        <v>867</v>
       </c>
       <c r="H166" s="1" t="s">
-        <v>888</v>
+        <v>480</v>
       </c>
       <c r="I166" s="1" t="s">
         <v>72</v>
@@ -10596,26 +10597,34 @@
       <c r="M166" s="1"/>
       <c r="N166" s="1"/>
       <c r="O166" s="1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="167" spans="1:15" x14ac:dyDescent="0.35">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="167" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A167">
-        <v>220</v>
+        <v>204</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>889</v>
+        <v>481</v>
       </c>
       <c r="C167" s="1" t="s">
-        <v>485</v>
+        <v>471</v>
       </c>
       <c r="D167" s="1" t="s">
-        <v>486</v>
+        <v>472</v>
+      </c>
+      <c r="E167" t="s">
+        <v>482</v>
       </c>
       <c r="F167" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H167" s="1"/>
+      <c r="G167" t="s">
+        <v>868</v>
+      </c>
+      <c r="H167" s="1" t="s">
+        <v>483</v>
+      </c>
       <c r="I167" s="1" t="s">
         <v>72</v>
       </c>
@@ -10627,15 +10636,15 @@
       <c r="M167" s="1"/>
       <c r="N167" s="1"/>
       <c r="O167" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="168" spans="1:15" x14ac:dyDescent="0.35">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="168" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A168">
-        <v>221</v>
+        <v>205</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>890</v>
+        <v>484</v>
       </c>
       <c r="C168" s="1" t="s">
         <v>485</v>
@@ -10644,16 +10653,16 @@
         <v>486</v>
       </c>
       <c r="E168" t="s">
-        <v>959</v>
+        <v>487</v>
       </c>
       <c r="F168" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G168" t="s">
-        <v>958</v>
+        <v>869</v>
       </c>
       <c r="H168" s="1" t="s">
-        <v>960</v>
+        <v>488</v>
       </c>
       <c r="I168" s="1" t="s">
         <v>72</v>
@@ -10666,31 +10675,33 @@
       <c r="M168" s="1"/>
       <c r="N168" s="1"/>
       <c r="O168" s="1" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="169" spans="1:15" x14ac:dyDescent="0.35">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="169" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A169">
-        <v>301</v>
+        <v>206</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>513</v>
+        <v>489</v>
       </c>
       <c r="C169" s="1" t="s">
-        <v>514</v>
+        <v>485</v>
       </c>
       <c r="D169" s="1" t="s">
-        <v>514</v>
-      </c>
-      <c r="E169" s="1" t="s">
-        <v>514</v>
+        <v>486</v>
+      </c>
+      <c r="E169" t="s">
+        <v>490</v>
       </c>
       <c r="F169" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G169" s="1"/>
+      <c r="G169" t="s">
+        <v>870</v>
+      </c>
       <c r="H169" s="1" t="s">
-        <v>515</v>
+        <v>491</v>
       </c>
       <c r="I169" s="1" t="s">
         <v>72</v>
@@ -10703,6 +10714,620 @@
       <c r="M169" s="1"/>
       <c r="N169" s="1"/>
       <c r="O169" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="170" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A170">
+        <v>207</v>
+      </c>
+      <c r="B170" s="1" t="s">
+        <v>492</v>
+      </c>
+      <c r="C170" s="1" t="s">
+        <v>485</v>
+      </c>
+      <c r="D170" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="E170" t="s">
+        <v>493</v>
+      </c>
+      <c r="F170" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G170" t="s">
+        <v>871</v>
+      </c>
+      <c r="H170" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="I170" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J170" s="1"/>
+      <c r="K170" s="1"/>
+      <c r="L170" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="M170" s="1"/>
+      <c r="N170" s="1"/>
+      <c r="O170" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="171" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A171">
+        <v>208</v>
+      </c>
+      <c r="B171" s="1" t="s">
+        <v>495</v>
+      </c>
+      <c r="C171" s="1" t="s">
+        <v>485</v>
+      </c>
+      <c r="D171" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="E171" t="s">
+        <v>496</v>
+      </c>
+      <c r="F171" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G171" t="s">
+        <v>872</v>
+      </c>
+      <c r="H171" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="I171" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J171" s="1"/>
+      <c r="K171" s="1"/>
+      <c r="L171" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="M171" s="1"/>
+      <c r="N171" s="1"/>
+      <c r="O171" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="172" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A172">
+        <v>209</v>
+      </c>
+      <c r="B172" s="1" t="s">
+        <v>498</v>
+      </c>
+      <c r="C172" s="1" t="s">
+        <v>485</v>
+      </c>
+      <c r="D172" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="E172" t="s">
+        <v>499</v>
+      </c>
+      <c r="F172" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G172" t="s">
+        <v>873</v>
+      </c>
+      <c r="H172" s="1" t="s">
+        <v>500</v>
+      </c>
+      <c r="I172" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J172" s="1"/>
+      <c r="K172" s="1"/>
+      <c r="L172" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="M172" s="1"/>
+      <c r="N172" s="1"/>
+      <c r="O172" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="173" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A173">
+        <v>210</v>
+      </c>
+      <c r="B173" s="1" t="s">
+        <v>501</v>
+      </c>
+      <c r="C173" s="1" t="s">
+        <v>485</v>
+      </c>
+      <c r="D173" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="E173" t="s">
+        <v>676</v>
+      </c>
+      <c r="F173" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G173" t="s">
+        <v>874</v>
+      </c>
+      <c r="H173" s="1" t="s">
+        <v>502</v>
+      </c>
+      <c r="I173" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J173" s="1"/>
+      <c r="K173" s="1"/>
+      <c r="L173" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="M173" s="1"/>
+      <c r="N173" s="1"/>
+      <c r="O173" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="174" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A174">
+        <v>211</v>
+      </c>
+      <c r="B174" s="1" t="s">
+        <v>503</v>
+      </c>
+      <c r="C174" s="1" t="s">
+        <v>485</v>
+      </c>
+      <c r="D174" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="E174" t="s">
+        <v>677</v>
+      </c>
+      <c r="F174" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G174" t="s">
+        <v>875</v>
+      </c>
+      <c r="H174" s="1" t="s">
+        <v>504</v>
+      </c>
+      <c r="I174" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J174" s="1"/>
+      <c r="K174" s="1"/>
+      <c r="L174" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="M174" s="1"/>
+      <c r="N174" s="1"/>
+      <c r="O174" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="175" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A175">
+        <v>212</v>
+      </c>
+      <c r="B175" s="1" t="s">
+        <v>505</v>
+      </c>
+      <c r="C175" s="1" t="s">
+        <v>485</v>
+      </c>
+      <c r="D175" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="E175" t="s">
+        <v>678</v>
+      </c>
+      <c r="F175" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G175" t="s">
+        <v>876</v>
+      </c>
+      <c r="H175" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="I175" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J175" s="1"/>
+      <c r="K175" s="1"/>
+      <c r="L175" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="M175" s="1"/>
+      <c r="N175" s="1"/>
+      <c r="O175" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="176" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A176">
+        <v>213</v>
+      </c>
+      <c r="B176" s="1" t="s">
+        <v>507</v>
+      </c>
+      <c r="C176" s="1" t="s">
+        <v>485</v>
+      </c>
+      <c r="D176" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="E176" t="s">
+        <v>508</v>
+      </c>
+      <c r="F176" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G176" t="s">
+        <v>877</v>
+      </c>
+      <c r="H176" s="1" t="s">
+        <v>509</v>
+      </c>
+      <c r="I176" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J176" s="1"/>
+      <c r="K176" s="1"/>
+      <c r="L176" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="M176" s="1"/>
+      <c r="N176" s="1"/>
+      <c r="O176" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="177" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A177">
+        <v>214</v>
+      </c>
+      <c r="B177" s="1" t="s">
+        <v>510</v>
+      </c>
+      <c r="C177" s="1" t="s">
+        <v>485</v>
+      </c>
+      <c r="D177" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="E177" t="s">
+        <v>511</v>
+      </c>
+      <c r="F177" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G177" t="s">
+        <v>878</v>
+      </c>
+      <c r="H177" s="1" t="s">
+        <v>512</v>
+      </c>
+      <c r="I177" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J177" s="1"/>
+      <c r="K177" s="1"/>
+      <c r="L177" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="M177" s="1"/>
+      <c r="N177" s="1"/>
+      <c r="O177" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="178" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A178">
+        <v>215</v>
+      </c>
+      <c r="B178" s="1" t="s">
+        <v>539</v>
+      </c>
+      <c r="C178" s="1" t="s">
+        <v>485</v>
+      </c>
+      <c r="D178" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="E178" t="s">
+        <v>544</v>
+      </c>
+      <c r="F178" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G178" t="s">
+        <v>879</v>
+      </c>
+      <c r="H178" s="1" t="s">
+        <v>880</v>
+      </c>
+      <c r="I178" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J178" s="1"/>
+      <c r="K178" s="1"/>
+      <c r="L178" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="M178" s="1"/>
+      <c r="N178" s="1"/>
+      <c r="O178" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="179" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A179">
+        <v>216</v>
+      </c>
+      <c r="B179" s="1" t="s">
+        <v>540</v>
+      </c>
+      <c r="C179" s="1" t="s">
+        <v>485</v>
+      </c>
+      <c r="D179" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="E179" t="s">
+        <v>545</v>
+      </c>
+      <c r="F179" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G179" t="s">
+        <v>881</v>
+      </c>
+      <c r="H179" s="1" t="s">
+        <v>882</v>
+      </c>
+      <c r="I179" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J179" s="1"/>
+      <c r="K179" s="1"/>
+      <c r="L179" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="M179" s="1"/>
+      <c r="N179" s="1"/>
+      <c r="O179" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="180" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A180">
+        <v>217</v>
+      </c>
+      <c r="B180" s="1" t="s">
+        <v>541</v>
+      </c>
+      <c r="C180" s="1" t="s">
+        <v>485</v>
+      </c>
+      <c r="D180" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="E180" t="s">
+        <v>679</v>
+      </c>
+      <c r="F180" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G180" t="s">
+        <v>883</v>
+      </c>
+      <c r="H180" s="1" t="s">
+        <v>884</v>
+      </c>
+      <c r="I180" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J180" s="1"/>
+      <c r="K180" s="1"/>
+      <c r="L180" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="M180" s="1"/>
+      <c r="N180" s="1"/>
+      <c r="O180" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="181" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A181">
+        <v>218</v>
+      </c>
+      <c r="B181" s="1" t="s">
+        <v>542</v>
+      </c>
+      <c r="C181" s="1" t="s">
+        <v>485</v>
+      </c>
+      <c r="D181" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="E181" t="s">
+        <v>680</v>
+      </c>
+      <c r="F181" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G181" t="s">
+        <v>885</v>
+      </c>
+      <c r="H181" s="1" t="s">
+        <v>886</v>
+      </c>
+      <c r="I181" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J181" s="1"/>
+      <c r="K181" s="1"/>
+      <c r="L181" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="M181" s="1"/>
+      <c r="N181" s="1"/>
+      <c r="O181" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="182" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A182">
+        <v>219</v>
+      </c>
+      <c r="B182" s="1" t="s">
+        <v>543</v>
+      </c>
+      <c r="C182" s="1" t="s">
+        <v>485</v>
+      </c>
+      <c r="D182" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="E182" t="s">
+        <v>546</v>
+      </c>
+      <c r="F182" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G182" t="s">
+        <v>887</v>
+      </c>
+      <c r="H182" s="1" t="s">
+        <v>888</v>
+      </c>
+      <c r="I182" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J182" s="1"/>
+      <c r="K182" s="1"/>
+      <c r="L182" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="M182" s="1"/>
+      <c r="N182" s="1"/>
+      <c r="O182" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="183" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A183">
+        <v>220</v>
+      </c>
+      <c r="B183" s="1" t="s">
+        <v>889</v>
+      </c>
+      <c r="C183" s="1" t="s">
+        <v>485</v>
+      </c>
+      <c r="D183" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="F183" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H183" s="1"/>
+      <c r="I183" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J183" s="1"/>
+      <c r="K183" s="1"/>
+      <c r="L183" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="M183" s="1"/>
+      <c r="N183" s="1"/>
+      <c r="O183" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="184" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A184">
+        <v>221</v>
+      </c>
+      <c r="B184" s="1" t="s">
+        <v>890</v>
+      </c>
+      <c r="C184" s="1" t="s">
+        <v>485</v>
+      </c>
+      <c r="D184" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="E184" t="s">
+        <v>959</v>
+      </c>
+      <c r="F184" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G184" t="s">
+        <v>958</v>
+      </c>
+      <c r="H184" s="1" t="s">
+        <v>960</v>
+      </c>
+      <c r="I184" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J184" s="1"/>
+      <c r="K184" s="1"/>
+      <c r="L184" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="M184" s="1"/>
+      <c r="N184" s="1"/>
+      <c r="O184" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="185" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A185">
+        <v>301</v>
+      </c>
+      <c r="B185" s="1" t="s">
+        <v>513</v>
+      </c>
+      <c r="C185" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="D185" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="E185" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="F185" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G185" s="1"/>
+      <c r="H185" s="1" t="s">
+        <v>515</v>
+      </c>
+      <c r="I185" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J185" s="1"/>
+      <c r="K185" s="1"/>
+      <c r="L185" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="M185" s="1"/>
+      <c r="N185" s="1"/>
+      <c r="O185" s="1" t="s">
         <v>144</v>
       </c>
     </row>

</xml_diff>